<commit_message>
fix GM#1.9 and finish GM#1.10
</commit_message>
<xml_diff>
--- a/SpaghettiTests.xlsx
+++ b/SpaghettiTests.xlsx
@@ -284,33 +284,33 @@
   </definedNames>
   <calcPr calcId="114210"/>
   <customWorkbookViews>
+    <customWorkbookView name="iryna_tsvirko - Personal View" guid="{D6B20FFB-1E0B-461B-BCA5-479EC9916837}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="555" tabRatio="602" activeSheetId="4"/>
+    <customWorkbookView name="Anastasiya_Hiliova - Personal View" guid="{CD7B856B-9EDA-43C8-96C4-9EE3BFC6A1C7}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="592" tabRatio="602" activeSheetId="4"/>
+    <customWorkbookView name="Tatsiana Aleksina - Personal View" guid="{83803FE8-F026-4EB6-8AA8-850C4281E75D}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="588" tabRatio="602" activeSheetId="4"/>
+    <customWorkbookView name="Kathleen Walsh - Personal View" guid="{6C7C9A60-7A7A-4C49-B916-23929D5F2F41}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="643" tabRatio="602" activeSheetId="4" showFormulaBar="0"/>
+    <customWorkbookView name="Siarhei_Varanovich - Personal View" guid="{6243D704-9E25-11D6-9C67-009027ED19E6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="592" tabRatio="602" activeSheetId="3"/>
+    <customWorkbookView name="Siarhei_Serko - Personal View" guid="{CC0CF5D6-B18D-491A-9FC9-FEBD5F8814E3}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="580" tabRatio="608" activeSheetId="3"/>
+    <customWorkbookView name="Yuliya_Huziy - Personal View" guid="{FEF12470-2E23-407A-98E1-8AB431BD4F04}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="553" tabRatio="602" activeSheetId="4"/>
+    <customWorkbookView name="Alexandr Belousov - Personal View" guid="{EB2A7A54-3035-4A67-821E-790B1FA9CB17}" mergeInterval="0" personalView="1" maximized="1" xWindow="4" yWindow="100" windowWidth="1012" windowHeight="576" activeSheetId="3"/>
+    <customWorkbookView name="Andrei Kulabukhau - Personal View" guid="{4CB4A757-2DE4-4B10-9E8C-5353D1A72D98}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="579" activeSheetId="6"/>
+    <customWorkbookView name="Igor Kalnik - Personal View" guid="{ECDB2518-881D-11D6-91C5-00A0C96BDFA3}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="605" activeSheetId="3"/>
+    <customWorkbookView name="Tatsiana Bohush - Personal View" guid="{7BBCACAA-43E1-40B6-ADAE-BB35DF313022}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="632" activeSheetId="6"/>
+    <customWorkbookView name="Aliaksandra  Ivanova - Personal View" guid="{2B891D42-6CB2-11D6-83C8-0003470A98B2}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="581" tabRatio="608" activeSheetId="2"/>
+    <customWorkbookView name="Volha Bahachuk - Personal View" guid="{38F36526-3D5C-4DDC-870E-899FBC48B66E}" mergeInterval="0" personalView="1" maximized="1" xWindow="2" yWindow="96" windowWidth="1020" windowHeight="603" activeSheetId="3"/>
+    <customWorkbookView name="Alena  Yermokhina - Personal View" guid="{5B8FA0FD-6C82-11D6-82E3-00A0C9A45549}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="580" activeSheetId="3" showComments="commIndAndComment"/>
+    <customWorkbookView name="Ruslan Mianzelen - Personal View" guid="{56D8F5D9-3A0D-4BF2-9433-8BEFE08B3700}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="554" activeSheetId="3"/>
+    <customWorkbookView name="Aliaksandra V. Ivanova - Personal View" guid="{EFAB871B-4EC1-40A1-9A59-7F13D3251E5D}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="607" activeSheetId="2"/>
+    <customWorkbookView name="Developer - Personal View" guid="{F21FA1CE-8CDC-4011-8CB5-DD27B77A6F07}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="579" activeSheetId="7"/>
+    <customWorkbookView name="Aliaksandr Mamus - Personal View" guid="{FFC053D9-391A-4F3D-A4C4-D8F3DC5064CF}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1115" windowHeight="810" activeSheetId="3"/>
+    <customWorkbookView name="Pavel Drachuk - Personal View" guid="{3EDD5E41-79E4-11D6-8216-009027651E6D}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="581" activeSheetId="2"/>
+    <customWorkbookView name="Siarhei Varanovich - Personal View" guid="{33D53BDF-065D-44AA-B0C7-519973E98EF8}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="605" tabRatio="602" activeSheetId="3"/>
+    <customWorkbookView name="Tatsiana Alexina - Personal View" guid="{D717C572-E042-4CE9-8903-02D390043ABD}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="580" tabRatio="602" activeSheetId="3"/>
+    <customWorkbookView name="Andrei Savastsiuk - Personal View" guid="{E55FF256-6BD4-11D6-8424-009027ED1955}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="570" activeSheetId="3"/>
+    <customWorkbookView name="Andrei_Savastsiuk - Personal View" guid="{C303A572-AC36-442D-BA31-03981F899203}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="562" tabRatio="602" activeSheetId="1"/>
+    <customWorkbookView name="Dzmitry_Bachkarou - Personal View" guid="{C28FB00F-BF30-4FCE-8162-662CDD4F052E}" mergeInterval="0" personalView="1" maximized="1" windowWidth="868" windowHeight="577" tabRatio="602" activeSheetId="4"/>
+    <customWorkbookView name="Alena Yermokhina - Personal View" guid="{162B80D8-2A0E-434F-A609-2DA7C93548E1}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="859" tabRatio="602" activeSheetId="4"/>
+    <customWorkbookView name="Hanna_Shuminskaya - Personal View" guid="{7603C6CA-5974-4912-AE1D-2245B995DDB4}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="580" tabRatio="602" activeSheetId="4"/>
     <customWorkbookView name="Katsiaryna_Yarshova - Personal View" guid="{D003CDB4-53EF-48AC-A14B-1EF99DCC6613}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="813" tabRatio="602" activeSheetId="1"/>
-    <customWorkbookView name="Hanna_Shuminskaya - Personal View" guid="{7603C6CA-5974-4912-AE1D-2245B995DDB4}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="580" tabRatio="602" activeSheetId="4"/>
-    <customWorkbookView name="Alena Yermokhina - Personal View" guid="{162B80D8-2A0E-434F-A609-2DA7C93548E1}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="859" tabRatio="602" activeSheetId="4"/>
-    <customWorkbookView name="Dzmitry_Bachkarou - Personal View" guid="{C28FB00F-BF30-4FCE-8162-662CDD4F052E}" mergeInterval="0" personalView="1" maximized="1" windowWidth="868" windowHeight="577" tabRatio="602" activeSheetId="4"/>
-    <customWorkbookView name="Andrei_Savastsiuk - Personal View" guid="{C303A572-AC36-442D-BA31-03981F899203}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="562" tabRatio="602" activeSheetId="1"/>
-    <customWorkbookView name="Andrei Savastsiuk - Personal View" guid="{E55FF256-6BD4-11D6-8424-009027ED1955}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="570" activeSheetId="3"/>
-    <customWorkbookView name="Tatsiana Alexina - Personal View" guid="{D717C572-E042-4CE9-8903-02D390043ABD}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="580" tabRatio="602" activeSheetId="3"/>
-    <customWorkbookView name="Siarhei Varanovich - Personal View" guid="{33D53BDF-065D-44AA-B0C7-519973E98EF8}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="605" tabRatio="602" activeSheetId="3"/>
-    <customWorkbookView name="Pavel Drachuk - Personal View" guid="{3EDD5E41-79E4-11D6-8216-009027651E6D}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="581" activeSheetId="2"/>
-    <customWorkbookView name="Aliaksandr Mamus - Personal View" guid="{FFC053D9-391A-4F3D-A4C4-D8F3DC5064CF}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1115" windowHeight="810" activeSheetId="3"/>
-    <customWorkbookView name="Developer - Personal View" guid="{F21FA1CE-8CDC-4011-8CB5-DD27B77A6F07}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="579" activeSheetId="7"/>
-    <customWorkbookView name="Aliaksandra V. Ivanova - Personal View" guid="{EFAB871B-4EC1-40A1-9A59-7F13D3251E5D}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="607" activeSheetId="2"/>
-    <customWorkbookView name="Ruslan Mianzelen - Personal View" guid="{56D8F5D9-3A0D-4BF2-9433-8BEFE08B3700}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="554" activeSheetId="3"/>
-    <customWorkbookView name="Alena  Yermokhina - Personal View" guid="{5B8FA0FD-6C82-11D6-82E3-00A0C9A45549}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="580" activeSheetId="3" showComments="commIndAndComment"/>
-    <customWorkbookView name="Volha Bahachuk - Personal View" guid="{38F36526-3D5C-4DDC-870E-899FBC48B66E}" mergeInterval="0" personalView="1" maximized="1" xWindow="2" yWindow="96" windowWidth="1020" windowHeight="603" activeSheetId="3"/>
-    <customWorkbookView name="Aliaksandra  Ivanova - Personal View" guid="{2B891D42-6CB2-11D6-83C8-0003470A98B2}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="581" tabRatio="608" activeSheetId="2"/>
-    <customWorkbookView name="Tatsiana Bohush - Personal View" guid="{7BBCACAA-43E1-40B6-ADAE-BB35DF313022}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="632" activeSheetId="6"/>
-    <customWorkbookView name="Igor Kalnik - Personal View" guid="{ECDB2518-881D-11D6-91C5-00A0C96BDFA3}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="605" activeSheetId="3"/>
-    <customWorkbookView name="Andrei Kulabukhau - Personal View" guid="{4CB4A757-2DE4-4B10-9E8C-5353D1A72D98}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="579" activeSheetId="6"/>
-    <customWorkbookView name="Alexandr Belousov - Personal View" guid="{EB2A7A54-3035-4A67-821E-790B1FA9CB17}" mergeInterval="0" personalView="1" maximized="1" xWindow="4" yWindow="100" windowWidth="1012" windowHeight="576" activeSheetId="3"/>
-    <customWorkbookView name="Yuliya_Huziy - Personal View" guid="{FEF12470-2E23-407A-98E1-8AB431BD4F04}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="553" tabRatio="602" activeSheetId="4"/>
-    <customWorkbookView name="Siarhei_Serko - Personal View" guid="{CC0CF5D6-B18D-491A-9FC9-FEBD5F8814E3}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="580" tabRatio="608" activeSheetId="3"/>
-    <customWorkbookView name="Siarhei_Varanovich - Personal View" guid="{6243D704-9E25-11D6-9C67-009027ED19E6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="592" tabRatio="602" activeSheetId="3"/>
-    <customWorkbookView name="Kathleen Walsh - Personal View" guid="{6C7C9A60-7A7A-4C49-B916-23929D5F2F41}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="643" tabRatio="602" activeSheetId="4" showFormulaBar="0"/>
-    <customWorkbookView name="Tatsiana Aleksina - Personal View" guid="{83803FE8-F026-4EB6-8AA8-850C4281E75D}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="588" tabRatio="602" activeSheetId="4"/>
-    <customWorkbookView name="Anastasiya_Hiliova - Personal View" guid="{CD7B856B-9EDA-43C8-96C4-9EE3BFC6A1C7}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="592" tabRatio="602" activeSheetId="4"/>
-    <customWorkbookView name="iryna_tsvirko - Personal View" guid="{D6B20FFB-1E0B-461B-BCA5-479EC9916837}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="555" tabRatio="602" activeSheetId="4"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -1145,7 +1145,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1415,6 +1415,9 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1927,80 +1930,80 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{D003CDB4-53EF-48AC-A14B-1EF99DCC6613}" showRuler="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <customSheetView guid="{D6B20FFB-1E0B-461B-BCA5-479EC9916837}" showRuler="0">
+      <selection activeCell="B13" sqref="B13"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{7603C6CA-5974-4912-AE1D-2245B995DDB4}" showRuler="0">
+    <customSheetView guid="{CD7B856B-9EDA-43C8-96C4-9EE3BFC6A1C7}" showRuler="0">
       <selection activeCell="B13" sqref="B13"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{162B80D8-2A0E-434F-A609-2DA7C93548E1}" showRuler="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <customSheetView guid="{83803FE8-F026-4EB6-8AA8-850C4281E75D}" showRuler="0">
+      <selection activeCell="B16" sqref="B16"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{C28FB00F-BF30-4FCE-8162-662CDD4F052E}" showRuler="0">
+    <customSheetView guid="{6C7C9A60-7A7A-4C49-B916-23929D5F2F41}" showRuler="0">
       <selection activeCell="B13" sqref="B13"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId4"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{C303A572-AC36-442D-BA31-03981F899203}" showRuler="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <customSheetView guid="{6243D704-9E25-11D6-9C67-009027ED19E6}" showRuler="0">
+      <selection activeCell="B12" sqref="B12"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId5"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{E55FF256-6BD4-11D6-8424-009027ED1955}" showPageBreaks="1" showRuler="0" topLeftCell="A4">
-      <selection activeCell="B12" sqref="B12"/>
+    <customSheetView guid="{CC0CF5D6-B18D-491A-9FC9-FEBD5F8814E3}" showRuler="0">
+      <selection activeCell="B9" sqref="B9"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup paperSize="9" orientation="landscape" r:id="rId6"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
-    <customSheetView guid="{D717C572-E042-4CE9-8903-02D390043ABD}" showRuler="0" topLeftCell="A4">
+      <pageSetup orientation="portrait" r:id="rId6"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
+    <customSheetView guid="{FEF12470-2E23-407A-98E1-8AB431BD4F04}" showRuler="0" topLeftCell="A4">
       <selection activeCell="B14" sqref="B14"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId7"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{33D53BDF-065D-44AA-B0C7-519973E98EF8}" showRuler="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <customSheetView guid="{EB2A7A54-3035-4A67-821E-790B1FA9CB17}" showPageBreaks="1" showRuler="0" topLeftCell="A4">
+      <selection activeCell="B3" sqref="B3"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId8"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{3EDD5E41-79E4-11D6-8216-009027651E6D}" showPageBreaks="1" showRuler="0">
-      <selection activeCell="C14" sqref="C14:C15"/>
+    <customSheetView guid="{4CB4A757-2DE4-4B10-9E8C-5353D1A72D98}" showRuler="0">
+      <selection activeCell="B12" sqref="B12"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId9"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{FFC053D9-391A-4F3D-A4C4-D8F3DC5064CF}" showRuler="0">
+    <customSheetView guid="{ECDB2518-881D-11D6-91C5-00A0C96BDFA3}" showRuler="0" topLeftCell="A10">
+      <selection activeCell="A9" sqref="A9"/>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <pageSetup orientation="portrait" r:id="rId10"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
+    <customSheetView guid="{7BBCACAA-43E1-40B6-ADAE-BB35DF313022}" showPageBreaks="1" showRuler="0" topLeftCell="A4">
+      <selection activeCell="B3" sqref="B3"/>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <pageSetup orientation="portrait" r:id="rId11"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
+    <customSheetView guid="{2B891D42-6CB2-11D6-83C8-0003470A98B2}" showPageBreaks="1" showRuler="0" topLeftCell="A10">
       <selection activeCell="B9" sqref="B9"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup orientation="portrait" r:id="rId10"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
-    <customSheetView guid="{F21FA1CE-8CDC-4011-8CB5-DD27B77A6F07}" showRuler="0">
-      <selection activeCell="B9" sqref="B9"/>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup orientation="portrait" r:id="rId11"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
-    <customSheetView guid="{EFAB871B-4EC1-40A1-9A59-7F13D3251E5D}" showPageBreaks="1" showRuler="0">
-      <selection activeCell="B12" sqref="B12"/>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId12"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{56D8F5D9-3A0D-4BF2-9433-8BEFE08B3700}" showRuler="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <customSheetView guid="{38F36526-3D5C-4DDC-870E-899FBC48B66E}" showRuler="0" topLeftCell="A10">
+      <selection activeCell="B13" sqref="B13"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId13"/>
       <headerFooter alignWithMargins="0"/>
@@ -2011,80 +2014,80 @@
       <pageSetup orientation="portrait" r:id="rId14"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{38F36526-3D5C-4DDC-870E-899FBC48B66E}" showRuler="0" topLeftCell="A10">
-      <selection activeCell="B13" sqref="B13"/>
+    <customSheetView guid="{56D8F5D9-3A0D-4BF2-9433-8BEFE08B3700}" showRuler="0">
+      <selection activeCell="B9" sqref="B9"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId15"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{2B891D42-6CB2-11D6-83C8-0003470A98B2}" showPageBreaks="1" showRuler="0" topLeftCell="A10">
+    <customSheetView guid="{EFAB871B-4EC1-40A1-9A59-7F13D3251E5D}" showPageBreaks="1" showRuler="0">
+      <selection activeCell="B12" sqref="B12"/>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <pageSetup orientation="portrait" r:id="rId16"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
+    <customSheetView guid="{F21FA1CE-8CDC-4011-8CB5-DD27B77A6F07}" showRuler="0">
       <selection activeCell="B9" sqref="B9"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup orientation="portrait" r:id="rId16"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
-    <customSheetView guid="{7BBCACAA-43E1-40B6-ADAE-BB35DF313022}" showPageBreaks="1" showRuler="0" topLeftCell="A4">
-      <selection activeCell="B3" sqref="B3"/>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId17"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{ECDB2518-881D-11D6-91C5-00A0C96BDFA3}" showRuler="0" topLeftCell="A10">
-      <selection activeCell="A9" sqref="A9"/>
+    <customSheetView guid="{FFC053D9-391A-4F3D-A4C4-D8F3DC5064CF}" showRuler="0">
+      <selection activeCell="B9" sqref="B9"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId18"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{4CB4A757-2DE4-4B10-9E8C-5353D1A72D98}" showRuler="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <customSheetView guid="{3EDD5E41-79E4-11D6-8216-009027651E6D}" showPageBreaks="1" showRuler="0">
+      <selection activeCell="C14" sqref="C14:C15"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId19"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{EB2A7A54-3035-4A67-821E-790B1FA9CB17}" showPageBreaks="1" showRuler="0" topLeftCell="A4">
-      <selection activeCell="B3" sqref="B3"/>
+    <customSheetView guid="{33D53BDF-065D-44AA-B0C7-519973E98EF8}" showRuler="0">
+      <selection activeCell="B10" sqref="B10"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId20"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{FEF12470-2E23-407A-98E1-8AB431BD4F04}" showRuler="0" topLeftCell="A4">
+    <customSheetView guid="{D717C572-E042-4CE9-8903-02D390043ABD}" showRuler="0" topLeftCell="A4">
       <selection activeCell="B14" sqref="B14"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId21"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{CC0CF5D6-B18D-491A-9FC9-FEBD5F8814E3}" showRuler="0">
-      <selection activeCell="B9" sqref="B9"/>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup orientation="portrait" r:id="rId22"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
-    <customSheetView guid="{6243D704-9E25-11D6-9C67-009027ED19E6}" showRuler="0">
+    <customSheetView guid="{E55FF256-6BD4-11D6-8424-009027ED1955}" showPageBreaks="1" showRuler="0" topLeftCell="A4">
       <selection activeCell="B12" sqref="B12"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <pageSetup paperSize="9" orientation="landscape" r:id="rId22"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
+    <customSheetView guid="{C303A572-AC36-442D-BA31-03981F899203}" showRuler="0">
+      <selection activeCell="A3" sqref="A3"/>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId23"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{6C7C9A60-7A7A-4C49-B916-23929D5F2F41}" showRuler="0">
+    <customSheetView guid="{C28FB00F-BF30-4FCE-8162-662CDD4F052E}" showRuler="0">
       <selection activeCell="B13" sqref="B13"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId24"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{83803FE8-F026-4EB6-8AA8-850C4281E75D}" showRuler="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <customSheetView guid="{162B80D8-2A0E-434F-A609-2DA7C93548E1}" showRuler="0">
+      <selection activeCell="B13" sqref="B13"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId25"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{CD7B856B-9EDA-43C8-96C4-9EE3BFC6A1C7}" showRuler="0">
+    <customSheetView guid="{7603C6CA-5974-4912-AE1D-2245B995DDB4}" showRuler="0">
       <selection activeCell="B13" sqref="B13"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId26"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{D6B20FFB-1E0B-461B-BCA5-479EC9916837}" showRuler="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <customSheetView guid="{D003CDB4-53EF-48AC-A14B-1EF99DCC6613}" showRuler="0">
+      <selection activeCell="B11" sqref="B11"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId27"/>
       <headerFooter alignWithMargins="0"/>
@@ -2105,8 +2108,8 @@
   </sheetPr>
   <dimension ref="A1:H80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="64" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="64" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -2688,81 +2691,81 @@
       <c r="F45" s="15"/>
     </row>
     <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A46" s="49"/>
-      <c r="B46" s="56"/>
-      <c r="C46" s="57"/>
-      <c r="D46" s="46" t="s">
+      <c r="A46" s="78"/>
+      <c r="B46" s="79"/>
+      <c r="C46" s="96"/>
+      <c r="D46" s="81" t="s">
         <v>93</v>
       </c>
-      <c r="E46" s="46"/>
+      <c r="E46" s="81"/>
       <c r="F46" s="15"/>
     </row>
     <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A47" s="49"/>
-      <c r="B47" s="56"/>
-      <c r="C47" s="57"/>
-      <c r="D47" s="46" t="s">
+      <c r="A47" s="78"/>
+      <c r="B47" s="79"/>
+      <c r="C47" s="96"/>
+      <c r="D47" s="81" t="s">
         <v>94</v>
       </c>
-      <c r="E47" s="46" t="s">
+      <c r="E47" s="81" t="s">
         <v>86</v>
       </c>
       <c r="F47" s="15"/>
     </row>
     <row r="48" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A48" s="49"/>
-      <c r="B48" s="56"/>
-      <c r="C48" s="57"/>
-      <c r="D48" s="46" t="s">
+      <c r="A48" s="78"/>
+      <c r="B48" s="79"/>
+      <c r="C48" s="96"/>
+      <c r="D48" s="81" t="s">
         <v>95</v>
       </c>
-      <c r="E48" s="46" t="s">
+      <c r="E48" s="81" t="s">
         <v>100</v>
       </c>
       <c r="F48" s="15"/>
     </row>
     <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A49" s="49"/>
-      <c r="B49" s="56"/>
-      <c r="C49" s="57"/>
-      <c r="D49" s="46" t="s">
+      <c r="A49" s="78"/>
+      <c r="B49" s="79"/>
+      <c r="C49" s="96"/>
+      <c r="D49" s="81" t="s">
         <v>96</v>
       </c>
-      <c r="E49" s="46" t="s">
+      <c r="E49" s="81" t="s">
         <v>101</v>
       </c>
       <c r="F49" s="15"/>
     </row>
     <row r="50" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A50" s="49"/>
-      <c r="B50" s="56"/>
-      <c r="C50" s="57"/>
-      <c r="D50" s="46" t="s">
+      <c r="A50" s="78"/>
+      <c r="B50" s="79"/>
+      <c r="C50" s="96"/>
+      <c r="D50" s="81" t="s">
         <v>97</v>
       </c>
-      <c r="E50" s="54"/>
+      <c r="E50" s="89"/>
       <c r="F50" s="15"/>
     </row>
     <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A51" s="49"/>
-      <c r="B51" s="56"/>
-      <c r="C51" s="57"/>
-      <c r="D51" s="46" t="s">
+      <c r="A51" s="78"/>
+      <c r="B51" s="79"/>
+      <c r="C51" s="96"/>
+      <c r="D51" s="81" t="s">
         <v>98</v>
       </c>
-      <c r="E51" s="46" t="s">
+      <c r="E51" s="81" t="s">
         <v>102</v>
       </c>
       <c r="F51" s="15"/>
     </row>
     <row r="52" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A52" s="49"/>
-      <c r="B52" s="56"/>
-      <c r="C52" s="57"/>
-      <c r="D52" s="46" t="s">
+      <c r="A52" s="78"/>
+      <c r="B52" s="79"/>
+      <c r="C52" s="96"/>
+      <c r="D52" s="81" t="s">
         <v>99</v>
       </c>
-      <c r="E52" s="46"/>
+      <c r="E52" s="81"/>
       <c r="F52" s="15"/>
     </row>
     <row r="53" spans="1:6" ht="15" x14ac:dyDescent="0.2">
@@ -2780,69 +2783,69 @@
       <c r="F53" s="15"/>
     </row>
     <row r="54" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A54" s="49"/>
-      <c r="B54" s="56"/>
-      <c r="C54" s="57"/>
-      <c r="D54" s="46" t="s">
+      <c r="A54" s="78"/>
+      <c r="B54" s="79"/>
+      <c r="C54" s="96"/>
+      <c r="D54" s="81" t="s">
         <v>93</v>
       </c>
-      <c r="E54" s="46"/>
+      <c r="E54" s="81"/>
       <c r="F54" s="15"/>
     </row>
     <row r="55" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A55" s="49"/>
-      <c r="B55" s="56"/>
-      <c r="C55" s="57"/>
-      <c r="D55" s="46" t="s">
+      <c r="A55" s="78"/>
+      <c r="B55" s="79"/>
+      <c r="C55" s="96"/>
+      <c r="D55" s="81" t="s">
         <v>94</v>
       </c>
-      <c r="E55" s="46" t="s">
+      <c r="E55" s="81" t="s">
         <v>86</v>
       </c>
       <c r="F55" s="15"/>
     </row>
     <row r="56" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A56" s="49"/>
-      <c r="B56" s="56"/>
-      <c r="C56" s="57"/>
-      <c r="D56" s="46" t="s">
+      <c r="A56" s="78"/>
+      <c r="B56" s="79"/>
+      <c r="C56" s="96"/>
+      <c r="D56" s="81" t="s">
         <v>105</v>
       </c>
-      <c r="E56" s="46" t="s">
+      <c r="E56" s="81" t="s">
         <v>109</v>
       </c>
       <c r="F56" s="15"/>
     </row>
     <row r="57" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A57" s="49"/>
-      <c r="B57" s="56"/>
-      <c r="C57" s="57"/>
-      <c r="D57" s="46" t="s">
+      <c r="A57" s="78"/>
+      <c r="B57" s="79"/>
+      <c r="C57" s="96"/>
+      <c r="D57" s="81" t="s">
         <v>106</v>
       </c>
-      <c r="E57" s="46"/>
+      <c r="E57" s="81"/>
       <c r="F57" s="15"/>
     </row>
     <row r="58" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A58" s="49"/>
-      <c r="B58" s="56"/>
-      <c r="C58" s="57"/>
-      <c r="D58" s="46" t="s">
+      <c r="A58" s="78"/>
+      <c r="B58" s="79"/>
+      <c r="C58" s="96"/>
+      <c r="D58" s="81" t="s">
         <v>107</v>
       </c>
-      <c r="E58" s="46" t="s">
+      <c r="E58" s="81" t="s">
         <v>110</v>
       </c>
       <c r="F58" s="15"/>
     </row>
     <row r="59" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A59" s="49"/>
-      <c r="B59" s="56"/>
-      <c r="C59" s="57"/>
-      <c r="D59" s="46" t="s">
+      <c r="A59" s="78"/>
+      <c r="B59" s="79"/>
+      <c r="C59" s="96"/>
+      <c r="D59" s="81" t="s">
         <v>108</v>
       </c>
-      <c r="E59" s="54"/>
+      <c r="E59" s="89"/>
       <c r="F59" s="15"/>
     </row>
     <row r="60" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3062,7 +3065,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{D003CDB4-53EF-48AC-A14B-1EF99DCC6613}" showAutoFilter="1" showRuler="0" topLeftCell="A142">
+    <customSheetView guid="{D6B20FFB-1E0B-461B-BCA5-479EC9916837}" showAutoFilter="1" hiddenRows="1" showRuler="0" topLeftCell="A142">
       <selection activeCell="A142" sqref="A142"/>
       <colBreaks count="5" manualBreakCount="5">
         <brk id="5" max="1048575" man="1"/>
@@ -3076,8 +3079,8 @@
       <headerFooter alignWithMargins="0"/>
       <autoFilter ref="B1:I1"/>
     </customSheetView>
-    <customSheetView guid="{7603C6CA-5974-4912-AE1D-2245B995DDB4}" showAutoFilter="1" hiddenRows="1" showRuler="0" topLeftCell="A142">
-      <selection activeCell="A142" sqref="A142"/>
+    <customSheetView guid="{CD7B856B-9EDA-43C8-96C4-9EE3BFC6A1C7}" showAutoFilter="1" showRuler="0" topLeftCell="A74">
+      <selection activeCell="A98" sqref="A98"/>
       <colBreaks count="5" manualBreakCount="5">
         <brk id="5" max="1048575" man="1"/>
         <brk id="8" max="1048575" man="1"/>
@@ -3090,8 +3093,8 @@
       <headerFooter alignWithMargins="0"/>
       <autoFilter ref="B1:I1"/>
     </customSheetView>
-    <customSheetView guid="{162B80D8-2A0E-434F-A609-2DA7C93548E1}" showAutoFilter="1" showRuler="0" topLeftCell="A74">
-      <selection activeCell="A98" sqref="A98"/>
+    <customSheetView guid="{83803FE8-F026-4EB6-8AA8-850C4281E75D}" showAutoFilter="1" hiddenRows="1" showRuler="0" topLeftCell="A5">
+      <selection activeCell="D184" sqref="D184"/>
       <colBreaks count="5" manualBreakCount="5">
         <brk id="5" max="1048575" man="1"/>
         <brk id="8" max="1048575" man="1"/>
@@ -3104,7 +3107,7 @@
       <headerFooter alignWithMargins="0"/>
       <autoFilter ref="B1:I1"/>
     </customSheetView>
-    <customSheetView guid="{C28FB00F-BF30-4FCE-8162-662CDD4F052E}" showAutoFilter="1" hiddenRows="1" showRuler="0" topLeftCell="A74">
+    <customSheetView guid="{6C7C9A60-7A7A-4C49-B916-23929D5F2F41}" showAutoFilter="1" showRuler="0" topLeftCell="A74">
       <selection activeCell="A98" sqref="A98"/>
       <colBreaks count="5" manualBreakCount="5">
         <brk id="5" max="1048575" man="1"/>
@@ -3118,8 +3121,8 @@
       <headerFooter alignWithMargins="0"/>
       <autoFilter ref="B1:I1"/>
     </customSheetView>
-    <customSheetView guid="{C303A572-AC36-442D-BA31-03981F899203}" showAutoFilter="1" hiddenRows="1" showRuler="0" topLeftCell="A4">
-      <selection activeCell="A213" sqref="A213"/>
+    <customSheetView guid="{6243D704-9E25-11D6-9C67-009027ED19E6}" showAutoFilter="1" hiddenRows="1" showRuler="0" topLeftCell="C26">
+      <selection activeCell="G45" sqref="G45"/>
       <colBreaks count="5" manualBreakCount="5">
         <brk id="5" max="1048575" man="1"/>
         <brk id="8" max="1048575" man="1"/>
@@ -3132,14 +3135,20 @@
       <headerFooter alignWithMargins="0"/>
       <autoFilter ref="B1:I1"/>
     </customSheetView>
-    <customSheetView guid="{E55FF256-6BD4-11D6-8424-009027ED1955}" showPageBreaks="1" hiddenRows="1" showRuler="0">
-      <selection activeCell="C7" sqref="C7"/>
-      <pageMargins left="0.23622047244094491" right="0" top="0.31496062992125984" bottom="0.23622047244094491" header="0.23622047244094491" footer="0.15748031496062992"/>
-      <pageSetup paperSize="9" orientation="landscape" r:id="rId6"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
-    <customSheetView guid="{D717C572-E042-4CE9-8903-02D390043ABD}" hiddenRows="1" showRuler="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <customSheetView guid="{CC0CF5D6-B18D-491A-9FC9-FEBD5F8814E3}" hiddenRows="1" showRuler="0" topLeftCell="A537">
+      <selection activeCell="C571" sqref="C571"/>
+      <colBreaks count="4" manualBreakCount="4">
+        <brk id="5" max="1048575" man="1"/>
+        <brk id="11" max="1048575" man="1"/>
+        <brk id="13" max="1048575" man="1"/>
+        <brk id="24" max="1048575" man="1"/>
+      </colBreaks>
+      <pageMargins left="0.25" right="0.17" top="0.32" bottom="0.25" header="0.22" footer="0.17"/>
+      <pageSetup orientation="portrait" r:id="rId6"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
+    <customSheetView guid="{FEF12470-2E23-407A-98E1-8AB431BD4F04}" hiddenRows="1" showRuler="0" topLeftCell="A221">
+      <selection activeCell="D701" sqref="D701"/>
       <colBreaks count="4" manualBreakCount="4">
         <brk id="5" max="1048575" man="1"/>
         <brk id="11" max="1048575" man="1"/>
@@ -3150,42 +3159,69 @@
       <pageSetup orientation="portrait" r:id="rId7"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{33D53BDF-065D-44AA-B0C7-519973E98EF8}" hiddenRows="1" showRuler="0" topLeftCell="A408">
-      <selection activeCell="A691" activeCellId="1" sqref="A690 A691"/>
-      <colBreaks count="4" manualBreakCount="4">
+    <customSheetView guid="{EB2A7A54-3035-4A67-821E-790B1FA9CB17}" scale="75" showPageBreaks="1" showRuler="0" topLeftCell="A826">
+      <selection activeCell="G830" sqref="G830"/>
+      <colBreaks count="6" manualBreakCount="6">
+        <brk id="5" max="1048575" man="1"/>
+        <brk id="9" max="1048575" man="1"/>
+        <brk id="11" max="1048575" man="1"/>
+        <brk id="13" max="1048575" man="1"/>
+        <brk id="24" max="1048575" man="1"/>
+        <brk id="35" max="1048575" man="1"/>
+      </colBreaks>
+      <pageMargins left="0.25" right="0.25" top="0.32" bottom="0.25" header="0.22" footer="0.17"/>
+      <pageSetup orientation="portrait" r:id="rId8"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
+    <customSheetView guid="{4CB4A757-2DE4-4B10-9E8C-5353D1A72D98}" scale="85" showRuler="0" topLeftCell="A763">
+      <selection activeCell="A1936" sqref="A1936:IV1936"/>
+      <colBreaks count="2" manualBreakCount="2">
+        <brk id="5" max="1048575" man="1"/>
+        <brk id="13" max="1048575" man="1"/>
+      </colBreaks>
+      <pageMargins left="0.25" right="0.25" top="0.32" bottom="0.25" header="0.22" footer="0.17"/>
+      <pageSetup orientation="portrait" r:id="rId9"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
+    <customSheetView guid="{ECDB2518-881D-11D6-91C5-00A0C96BDFA3}" hiddenRows="1" showRuler="0" topLeftCell="A9">
+      <selection activeCell="A1106" sqref="A1106"/>
+      <colBreaks count="3" manualBreakCount="3">
         <brk id="5" max="1048575" man="1"/>
         <brk id="11" max="1048575" man="1"/>
         <brk id="13" max="1048575" man="1"/>
-        <brk id="24" max="1048575" man="1"/>
-      </colBreaks>
-      <pageMargins left="0.25" right="0.25" top="0.32" bottom="0.25" header="0.22" footer="0.17"/>
-      <pageSetup orientation="portrait" r:id="rId8"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
-    <customSheetView guid="{3EDD5E41-79E4-11D6-8216-009027651E6D}" scale="75" showPageBreaks="1" hiddenRows="1" showRuler="0" topLeftCell="A822">
-      <selection activeCell="F836" sqref="F836"/>
-      <colBreaks count="5" manualBreakCount="5">
-        <brk id="5" max="1048575" man="1"/>
-        <brk id="6" max="1048575" man="1"/>
-        <brk id="10" max="1048575" man="1"/>
-        <brk id="12" max="1048575" man="1"/>
-        <brk id="16" max="1048575" man="1"/>
-      </colBreaks>
-      <pageMargins left="0.25" right="0.25" top="0.32" bottom="0.25" header="0.22" footer="0.17"/>
-      <pageSetup orientation="portrait" r:id="rId9"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
-    <customSheetView guid="{FFC053D9-391A-4F3D-A4C4-D8F3DC5064CF}" showRuler="0" topLeftCell="A279">
-      <selection activeCell="E286" sqref="E286"/>
-      <colBreaks count="1" manualBreakCount="1">
-        <brk id="5" max="1048575" man="1"/>
       </colBreaks>
       <pageMargins left="0.25" right="0.25" top="0.32" bottom="0.25" header="0.22" footer="0.17"/>
       <pageSetup orientation="portrait" r:id="rId10"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{F21FA1CE-8CDC-4011-8CB5-DD27B77A6F07}" showPageBreaks="1" showRuler="0" topLeftCell="A2502">
-      <selection activeCell="B2506" sqref="B2506"/>
+    <customSheetView guid="{7BBCACAA-43E1-40B6-ADAE-BB35DF313022}" showPageBreaks="1" showRuler="0" topLeftCell="A618">
+      <selection activeCell="H620" sqref="H620"/>
+      <colBreaks count="4" manualBreakCount="4">
+        <brk id="6" max="1048575" man="1"/>
+        <brk id="11" max="1048575" man="1"/>
+        <brk id="13" max="1048575" man="1"/>
+        <brk id="26" max="1048575" man="1"/>
+      </colBreaks>
+      <pageMargins left="0.25" right="0.25" top="0.32" bottom="0.25" header="0.22" footer="0.17"/>
+      <pageSetup scale="82" orientation="portrait" r:id="rId11"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
+    <customSheetView guid="{2B891D42-6CB2-11D6-83C8-0003470A98B2}" showPageBreaks="1" hiddenRows="1" showRuler="0" topLeftCell="A2301">
+      <selection activeCell="A2439" sqref="A2439:IV2439"/>
+      <colBreaks count="6" manualBreakCount="6">
+        <brk id="4" max="1048575" man="1"/>
+        <brk id="5" max="1048575" man="1"/>
+        <brk id="8" max="1048575" man="1"/>
+        <brk id="9" max="1048575" man="1"/>
+        <brk id="11" max="1048575" man="1"/>
+        <brk id="15" max="1048575" man="1"/>
+      </colBreaks>
+      <pageMargins left="0.25" right="0.25" top="0.32" bottom="0.25" header="0.22" footer="0.17"/>
+      <pageSetup orientation="portrait" r:id="rId12"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
+    <customSheetView guid="{38F36526-3D5C-4DDC-870E-899FBC48B66E}" hiddenRows="1" showRuler="0" topLeftCell="A2832">
+      <selection activeCell="C2833" sqref="C2833"/>
       <colBreaks count="5" manualBreakCount="5">
         <brk id="5" max="1048575" man="1"/>
         <brk id="9" max="1048575" man="1"/>
@@ -3194,57 +3230,8 @@
         <brk id="33" max="1048575" man="1"/>
       </colBreaks>
       <pageMargins left="0.25" right="0.25" top="0.32" bottom="0.25" header="0.22" footer="0.17"/>
-      <pageSetup orientation="portrait" r:id="rId11"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
-    <customSheetView guid="{EFAB871B-4EC1-40A1-9A59-7F13D3251E5D}" showPageBreaks="1" showRuler="0" topLeftCell="A2520">
-      <selection activeCell="A3027" sqref="A3027:IV3027"/>
-      <colBreaks count="5" manualBreakCount="5">
-        <brk id="3" max="1048575" man="1"/>
-        <brk id="4" max="1048575" man="1"/>
-        <brk id="8" max="1048575" man="1"/>
-        <brk id="10" max="1048575" man="1"/>
-        <brk id="12" max="1048575" man="1"/>
-      </colBreaks>
-      <pageMargins left="0.25" right="0.25" top="0.32" bottom="0.25" header="0.22" footer="0.17"/>
-      <pageSetup orientation="portrait" r:id="rId12"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
-    <customSheetView guid="{56D8F5D9-3A0D-4BF2-9433-8BEFE08B3700}" showPageBreaks="1" hiddenRows="1" showRuler="0" topLeftCell="A695">
-      <selection activeCell="D586" sqref="D586"/>
-      <colBreaks count="26" manualBreakCount="26">
-        <brk id="5" max="1048575" man="1"/>
-        <brk id="6" max="1048575" man="1"/>
-        <brk id="11" max="1048575" man="1"/>
-        <brk id="12" max="1048575" man="1"/>
-        <brk id="15" max="1048575" man="1"/>
-        <brk id="26" max="1992" man="1"/>
-        <brk id="37" max="1992" man="1"/>
-        <brk id="48" max="1992" man="1"/>
-        <brk id="59" max="1992" man="1"/>
-        <brk id="70" max="1992" man="1"/>
-        <brk id="81" max="1992" man="1"/>
-        <brk id="92" max="1992" man="1"/>
-        <brk id="103" max="1992" man="1"/>
-        <brk id="114" max="1992" man="1"/>
-        <brk id="125" max="1992" man="1"/>
-        <brk id="136" max="1992" man="1"/>
-        <brk id="147" max="1992" man="1"/>
-        <brk id="158" max="1992" man="1"/>
-        <brk id="169" max="1992" man="1"/>
-        <brk id="180" max="1992" man="1"/>
-        <brk id="191" max="1992" man="1"/>
-        <brk id="202" max="1992" man="1"/>
-        <brk id="213" max="1992" man="1"/>
-        <brk id="224" max="1992" man="1"/>
-        <brk id="235" max="1992" man="1"/>
-        <brk id="246" max="1992" man="1"/>
-      </colBreaks>
-      <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.31496062992125984" bottom="0.23622047244094491" header="0.15748031496062992" footer="0.15748031496062992"/>
       <pageSetup orientation="portrait" r:id="rId13"/>
-      <headerFooter alignWithMargins="0">
-        <oddHeader>&amp;L&amp;D&amp;R&amp;P</oddHeader>
-      </headerFooter>
+      <headerFooter alignWithMargins="0"/>
     </customSheetView>
     <customSheetView guid="{5B8FA0FD-6C82-11D6-82E3-00A0C9A45549}" showPageBreaks="1" hiddenRows="1" showRuler="0" topLeftCell="A1719">
       <selection activeCell="E1721" sqref="E1721"/>
@@ -3281,8 +3268,57 @@
         <oddHeader>&amp;L&amp;D&amp;R&amp;P</oddHeader>
       </headerFooter>
     </customSheetView>
-    <customSheetView guid="{38F36526-3D5C-4DDC-870E-899FBC48B66E}" hiddenRows="1" showRuler="0" topLeftCell="A2832">
-      <selection activeCell="C2833" sqref="C2833"/>
+    <customSheetView guid="{56D8F5D9-3A0D-4BF2-9433-8BEFE08B3700}" showPageBreaks="1" hiddenRows="1" showRuler="0" topLeftCell="A695">
+      <selection activeCell="D586" sqref="D586"/>
+      <colBreaks count="26" manualBreakCount="26">
+        <brk id="5" max="1048575" man="1"/>
+        <brk id="6" max="1048575" man="1"/>
+        <brk id="11" max="1048575" man="1"/>
+        <brk id="12" max="1048575" man="1"/>
+        <brk id="15" max="1048575" man="1"/>
+        <brk id="26" max="1992" man="1"/>
+        <brk id="37" max="1992" man="1"/>
+        <brk id="48" max="1992" man="1"/>
+        <brk id="59" max="1992" man="1"/>
+        <brk id="70" max="1992" man="1"/>
+        <brk id="81" max="1992" man="1"/>
+        <brk id="92" max="1992" man="1"/>
+        <brk id="103" max="1992" man="1"/>
+        <brk id="114" max="1992" man="1"/>
+        <brk id="125" max="1992" man="1"/>
+        <brk id="136" max="1992" man="1"/>
+        <brk id="147" max="1992" man="1"/>
+        <brk id="158" max="1992" man="1"/>
+        <brk id="169" max="1992" man="1"/>
+        <brk id="180" max="1992" man="1"/>
+        <brk id="191" max="1992" man="1"/>
+        <brk id="202" max="1992" man="1"/>
+        <brk id="213" max="1992" man="1"/>
+        <brk id="224" max="1992" man="1"/>
+        <brk id="235" max="1992" man="1"/>
+        <brk id="246" max="1992" man="1"/>
+      </colBreaks>
+      <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.31496062992125984" bottom="0.23622047244094491" header="0.15748031496062992" footer="0.15748031496062992"/>
+      <pageSetup orientation="portrait" r:id="rId15"/>
+      <headerFooter alignWithMargins="0">
+        <oddHeader>&amp;L&amp;D&amp;R&amp;P</oddHeader>
+      </headerFooter>
+    </customSheetView>
+    <customSheetView guid="{EFAB871B-4EC1-40A1-9A59-7F13D3251E5D}" showPageBreaks="1" showRuler="0" topLeftCell="A2520">
+      <selection activeCell="A3027" sqref="A3027:IV3027"/>
+      <colBreaks count="5" manualBreakCount="5">
+        <brk id="3" max="1048575" man="1"/>
+        <brk id="4" max="1048575" man="1"/>
+        <brk id="8" max="1048575" man="1"/>
+        <brk id="10" max="1048575" man="1"/>
+        <brk id="12" max="1048575" man="1"/>
+      </colBreaks>
+      <pageMargins left="0.25" right="0.25" top="0.32" bottom="0.25" header="0.22" footer="0.17"/>
+      <pageSetup orientation="portrait" r:id="rId16"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
+    <customSheetView guid="{F21FA1CE-8CDC-4011-8CB5-DD27B77A6F07}" showPageBreaks="1" showRuler="0" topLeftCell="A2502">
+      <selection activeCell="B2506" sqref="B2506"/>
       <colBreaks count="5" manualBreakCount="5">
         <brk id="5" max="1048575" man="1"/>
         <brk id="9" max="1048575" man="1"/>
@@ -3291,72 +3327,45 @@
         <brk id="33" max="1048575" man="1"/>
       </colBreaks>
       <pageMargins left="0.25" right="0.25" top="0.32" bottom="0.25" header="0.22" footer="0.17"/>
-      <pageSetup orientation="portrait" r:id="rId15"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
-    <customSheetView guid="{2B891D42-6CB2-11D6-83C8-0003470A98B2}" showPageBreaks="1" hiddenRows="1" showRuler="0" topLeftCell="A2301">
-      <selection activeCell="A2439" sqref="A2439:IV2439"/>
-      <colBreaks count="6" manualBreakCount="6">
-        <brk id="4" max="1048575" man="1"/>
+      <pageSetup orientation="portrait" r:id="rId17"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
+    <customSheetView guid="{FFC053D9-391A-4F3D-A4C4-D8F3DC5064CF}" showRuler="0" topLeftCell="A279">
+      <selection activeCell="E286" sqref="E286"/>
+      <colBreaks count="1" manualBreakCount="1">
         <brk id="5" max="1048575" man="1"/>
-        <brk id="8" max="1048575" man="1"/>
-        <brk id="9" max="1048575" man="1"/>
-        <brk id="11" max="1048575" man="1"/>
-        <brk id="15" max="1048575" man="1"/>
       </colBreaks>
       <pageMargins left="0.25" right="0.25" top="0.32" bottom="0.25" header="0.22" footer="0.17"/>
-      <pageSetup orientation="portrait" r:id="rId16"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
-    <customSheetView guid="{7BBCACAA-43E1-40B6-ADAE-BB35DF313022}" showPageBreaks="1" showRuler="0" topLeftCell="A618">
-      <selection activeCell="H620" sqref="H620"/>
-      <colBreaks count="4" manualBreakCount="4">
+      <pageSetup orientation="portrait" r:id="rId18"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
+    <customSheetView guid="{3EDD5E41-79E4-11D6-8216-009027651E6D}" scale="75" showPageBreaks="1" hiddenRows="1" showRuler="0" topLeftCell="A822">
+      <selection activeCell="F836" sqref="F836"/>
+      <colBreaks count="5" manualBreakCount="5">
+        <brk id="5" max="1048575" man="1"/>
         <brk id="6" max="1048575" man="1"/>
-        <brk id="11" max="1048575" man="1"/>
-        <brk id="13" max="1048575" man="1"/>
-        <brk id="26" max="1048575" man="1"/>
+        <brk id="10" max="1048575" man="1"/>
+        <brk id="12" max="1048575" man="1"/>
+        <brk id="16" max="1048575" man="1"/>
       </colBreaks>
       <pageMargins left="0.25" right="0.25" top="0.32" bottom="0.25" header="0.22" footer="0.17"/>
-      <pageSetup scale="82" orientation="portrait" r:id="rId17"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
-    <customSheetView guid="{ECDB2518-881D-11D6-91C5-00A0C96BDFA3}" hiddenRows="1" showRuler="0" topLeftCell="A9">
-      <selection activeCell="A1106" sqref="A1106"/>
-      <colBreaks count="3" manualBreakCount="3">
+      <pageSetup orientation="portrait" r:id="rId19"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
+    <customSheetView guid="{33D53BDF-065D-44AA-B0C7-519973E98EF8}" hiddenRows="1" showRuler="0" topLeftCell="A408">
+      <selection activeCell="A691" activeCellId="1" sqref="A690 A691"/>
+      <colBreaks count="4" manualBreakCount="4">
         <brk id="5" max="1048575" man="1"/>
         <brk id="11" max="1048575" man="1"/>
         <brk id="13" max="1048575" man="1"/>
-      </colBreaks>
-      <pageMargins left="0.25" right="0.25" top="0.32" bottom="0.25" header="0.22" footer="0.17"/>
-      <pageSetup orientation="portrait" r:id="rId18"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
-    <customSheetView guid="{4CB4A757-2DE4-4B10-9E8C-5353D1A72D98}" scale="85" showRuler="0" topLeftCell="A763">
-      <selection activeCell="A1936" sqref="A1936:IV1936"/>
-      <colBreaks count="2" manualBreakCount="2">
-        <brk id="5" max="1048575" man="1"/>
-        <brk id="13" max="1048575" man="1"/>
-      </colBreaks>
-      <pageMargins left="0.25" right="0.25" top="0.32" bottom="0.25" header="0.22" footer="0.17"/>
-      <pageSetup orientation="portrait" r:id="rId19"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
-    <customSheetView guid="{EB2A7A54-3035-4A67-821E-790B1FA9CB17}" scale="75" showPageBreaks="1" showRuler="0" topLeftCell="A826">
-      <selection activeCell="G830" sqref="G830"/>
-      <colBreaks count="6" manualBreakCount="6">
-        <brk id="5" max="1048575" man="1"/>
-        <brk id="9" max="1048575" man="1"/>
-        <brk id="11" max="1048575" man="1"/>
-        <brk id="13" max="1048575" man="1"/>
         <brk id="24" max="1048575" man="1"/>
-        <brk id="35" max="1048575" man="1"/>
       </colBreaks>
       <pageMargins left="0.25" right="0.25" top="0.32" bottom="0.25" header="0.22" footer="0.17"/>
       <pageSetup orientation="portrait" r:id="rId20"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{FEF12470-2E23-407A-98E1-8AB431BD4F04}" hiddenRows="1" showRuler="0" topLeftCell="A221">
-      <selection activeCell="D701" sqref="D701"/>
+    <customSheetView guid="{D717C572-E042-4CE9-8903-02D390043ABD}" hiddenRows="1" showRuler="0">
+      <selection activeCell="A7" sqref="A7"/>
       <colBreaks count="4" manualBreakCount="4">
         <brk id="5" max="1048575" man="1"/>
         <brk id="11" max="1048575" man="1"/>
@@ -3367,20 +3376,14 @@
       <pageSetup orientation="portrait" r:id="rId21"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{CC0CF5D6-B18D-491A-9FC9-FEBD5F8814E3}" hiddenRows="1" showRuler="0" topLeftCell="A537">
-      <selection activeCell="C571" sqref="C571"/>
-      <colBreaks count="4" manualBreakCount="4">
-        <brk id="5" max="1048575" man="1"/>
-        <brk id="11" max="1048575" man="1"/>
-        <brk id="13" max="1048575" man="1"/>
-        <brk id="24" max="1048575" man="1"/>
-      </colBreaks>
-      <pageMargins left="0.25" right="0.17" top="0.32" bottom="0.25" header="0.22" footer="0.17"/>
-      <pageSetup orientation="portrait" r:id="rId22"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
-    <customSheetView guid="{6243D704-9E25-11D6-9C67-009027ED19E6}" showAutoFilter="1" hiddenRows="1" showRuler="0" topLeftCell="C26">
-      <selection activeCell="G45" sqref="G45"/>
+    <customSheetView guid="{E55FF256-6BD4-11D6-8424-009027ED1955}" showPageBreaks="1" hiddenRows="1" showRuler="0">
+      <selection activeCell="C7" sqref="C7"/>
+      <pageMargins left="0.23622047244094491" right="0" top="0.31496062992125984" bottom="0.23622047244094491" header="0.23622047244094491" footer="0.15748031496062992"/>
+      <pageSetup paperSize="9" orientation="landscape" r:id="rId22"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
+    <customSheetView guid="{C303A572-AC36-442D-BA31-03981F899203}" showAutoFilter="1" hiddenRows="1" showRuler="0" topLeftCell="A4">
+      <selection activeCell="A213" sqref="A213"/>
       <colBreaks count="5" manualBreakCount="5">
         <brk id="5" max="1048575" man="1"/>
         <brk id="8" max="1048575" man="1"/>
@@ -3393,7 +3396,7 @@
       <headerFooter alignWithMargins="0"/>
       <autoFilter ref="B1:I1"/>
     </customSheetView>
-    <customSheetView guid="{6C7C9A60-7A7A-4C49-B916-23929D5F2F41}" showAutoFilter="1" showRuler="0" topLeftCell="A74">
+    <customSheetView guid="{C28FB00F-BF30-4FCE-8162-662CDD4F052E}" showAutoFilter="1" hiddenRows="1" showRuler="0" topLeftCell="A74">
       <selection activeCell="A98" sqref="A98"/>
       <colBreaks count="5" manualBreakCount="5">
         <brk id="5" max="1048575" man="1"/>
@@ -3407,8 +3410,8 @@
       <headerFooter alignWithMargins="0"/>
       <autoFilter ref="B1:I1"/>
     </customSheetView>
-    <customSheetView guid="{83803FE8-F026-4EB6-8AA8-850C4281E75D}" showAutoFilter="1" hiddenRows="1" showRuler="0" topLeftCell="A5">
-      <selection activeCell="D184" sqref="D184"/>
+    <customSheetView guid="{162B80D8-2A0E-434F-A609-2DA7C93548E1}" showAutoFilter="1" showRuler="0" topLeftCell="A74">
+      <selection activeCell="A98" sqref="A98"/>
       <colBreaks count="5" manualBreakCount="5">
         <brk id="5" max="1048575" man="1"/>
         <brk id="8" max="1048575" man="1"/>
@@ -3421,8 +3424,8 @@
       <headerFooter alignWithMargins="0"/>
       <autoFilter ref="B1:I1"/>
     </customSheetView>
-    <customSheetView guid="{CD7B856B-9EDA-43C8-96C4-9EE3BFC6A1C7}" showAutoFilter="1" showRuler="0" topLeftCell="A74">
-      <selection activeCell="A98" sqref="A98"/>
+    <customSheetView guid="{7603C6CA-5974-4912-AE1D-2245B995DDB4}" showAutoFilter="1" hiddenRows="1" showRuler="0" topLeftCell="A142">
+      <selection activeCell="A142" sqref="A142"/>
       <colBreaks count="5" manualBreakCount="5">
         <brk id="5" max="1048575" man="1"/>
         <brk id="8" max="1048575" man="1"/>
@@ -3435,7 +3438,7 @@
       <headerFooter alignWithMargins="0"/>
       <autoFilter ref="B1:I1"/>
     </customSheetView>
-    <customSheetView guid="{D6B20FFB-1E0B-461B-BCA5-479EC9916837}" showAutoFilter="1" hiddenRows="1" showRuler="0" topLeftCell="A142">
+    <customSheetView guid="{D003CDB4-53EF-48AC-A14B-1EF99DCC6613}" showAutoFilter="1" showRuler="0" topLeftCell="A142">
       <selection activeCell="A142" sqref="A142"/>
       <colBreaks count="5" manualBreakCount="5">
         <brk id="5" max="1048575" man="1"/>

</xml_diff>

<commit_message>
Refactoring. Create test classes. Create ConfirmationPage. Create enum of users
</commit_message>
<xml_diff>
--- a/SpaghettiTests.xlsx
+++ b/SpaghettiTests.xlsx
@@ -284,39 +284,39 @@
   </definedNames>
   <calcPr calcId="114210"/>
   <customWorkbookViews>
+    <customWorkbookView name="Katsiaryna_Yarshova - Personal View" guid="{D003CDB4-53EF-48AC-A14B-1EF99DCC6613}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="813" tabRatio="602" activeSheetId="1"/>
+    <customWorkbookView name="Hanna_Shuminskaya - Personal View" guid="{7603C6CA-5974-4912-AE1D-2245B995DDB4}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="580" tabRatio="602" activeSheetId="4"/>
+    <customWorkbookView name="Alena Yermokhina - Personal View" guid="{162B80D8-2A0E-434F-A609-2DA7C93548E1}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="859" tabRatio="602" activeSheetId="4"/>
+    <customWorkbookView name="Dzmitry_Bachkarou - Personal View" guid="{C28FB00F-BF30-4FCE-8162-662CDD4F052E}" mergeInterval="0" personalView="1" maximized="1" windowWidth="868" windowHeight="577" tabRatio="602" activeSheetId="4"/>
+    <customWorkbookView name="Andrei_Savastsiuk - Personal View" guid="{C303A572-AC36-442D-BA31-03981F899203}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="562" tabRatio="602" activeSheetId="1"/>
+    <customWorkbookView name="Andrei Savastsiuk - Personal View" guid="{E55FF256-6BD4-11D6-8424-009027ED1955}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="570" activeSheetId="3"/>
+    <customWorkbookView name="Tatsiana Alexina - Personal View" guid="{D717C572-E042-4CE9-8903-02D390043ABD}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="580" tabRatio="602" activeSheetId="3"/>
+    <customWorkbookView name="Siarhei Varanovich - Personal View" guid="{33D53BDF-065D-44AA-B0C7-519973E98EF8}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="605" tabRatio="602" activeSheetId="3"/>
+    <customWorkbookView name="Pavel Drachuk - Personal View" guid="{3EDD5E41-79E4-11D6-8216-009027651E6D}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="581" activeSheetId="2"/>
+    <customWorkbookView name="Aliaksandr Mamus - Personal View" guid="{FFC053D9-391A-4F3D-A4C4-D8F3DC5064CF}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1115" windowHeight="810" activeSheetId="3"/>
+    <customWorkbookView name="Developer - Personal View" guid="{F21FA1CE-8CDC-4011-8CB5-DD27B77A6F07}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="579" activeSheetId="7"/>
+    <customWorkbookView name="Aliaksandra V. Ivanova - Personal View" guid="{EFAB871B-4EC1-40A1-9A59-7F13D3251E5D}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="607" activeSheetId="2"/>
+    <customWorkbookView name="Ruslan Mianzelen - Personal View" guid="{56D8F5D9-3A0D-4BF2-9433-8BEFE08B3700}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="554" activeSheetId="3"/>
+    <customWorkbookView name="Alena  Yermokhina - Personal View" guid="{5B8FA0FD-6C82-11D6-82E3-00A0C9A45549}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="580" activeSheetId="3" showComments="commIndAndComment"/>
+    <customWorkbookView name="Volha Bahachuk - Personal View" guid="{38F36526-3D5C-4DDC-870E-899FBC48B66E}" mergeInterval="0" personalView="1" maximized="1" xWindow="2" yWindow="96" windowWidth="1020" windowHeight="603" activeSheetId="3"/>
+    <customWorkbookView name="Aliaksandra  Ivanova - Personal View" guid="{2B891D42-6CB2-11D6-83C8-0003470A98B2}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="581" tabRatio="608" activeSheetId="2"/>
+    <customWorkbookView name="Tatsiana Bohush - Personal View" guid="{7BBCACAA-43E1-40B6-ADAE-BB35DF313022}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="632" activeSheetId="6"/>
+    <customWorkbookView name="Igor Kalnik - Personal View" guid="{ECDB2518-881D-11D6-91C5-00A0C96BDFA3}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="605" activeSheetId="3"/>
+    <customWorkbookView name="Andrei Kulabukhau - Personal View" guid="{4CB4A757-2DE4-4B10-9E8C-5353D1A72D98}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="579" activeSheetId="6"/>
+    <customWorkbookView name="Alexandr Belousov - Personal View" guid="{EB2A7A54-3035-4A67-821E-790B1FA9CB17}" mergeInterval="0" personalView="1" maximized="1" xWindow="4" yWindow="100" windowWidth="1012" windowHeight="576" activeSheetId="3"/>
+    <customWorkbookView name="Yuliya_Huziy - Personal View" guid="{FEF12470-2E23-407A-98E1-8AB431BD4F04}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="553" tabRatio="602" activeSheetId="4"/>
+    <customWorkbookView name="Siarhei_Serko - Personal View" guid="{CC0CF5D6-B18D-491A-9FC9-FEBD5F8814E3}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="580" tabRatio="608" activeSheetId="3"/>
+    <customWorkbookView name="Siarhei_Varanovich - Personal View" guid="{6243D704-9E25-11D6-9C67-009027ED19E6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="592" tabRatio="602" activeSheetId="3"/>
+    <customWorkbookView name="Kathleen Walsh - Personal View" guid="{6C7C9A60-7A7A-4C49-B916-23929D5F2F41}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="643" tabRatio="602" activeSheetId="4" showFormulaBar="0"/>
+    <customWorkbookView name="Tatsiana Aleksina - Personal View" guid="{83803FE8-F026-4EB6-8AA8-850C4281E75D}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="588" tabRatio="602" activeSheetId="4"/>
+    <customWorkbookView name="Anastasiya_Hiliova - Personal View" guid="{CD7B856B-9EDA-43C8-96C4-9EE3BFC6A1C7}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="592" tabRatio="602" activeSheetId="4"/>
     <customWorkbookView name="iryna_tsvirko - Personal View" guid="{D6B20FFB-1E0B-461B-BCA5-479EC9916837}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="555" tabRatio="602" activeSheetId="4"/>
-    <customWorkbookView name="Anastasiya_Hiliova - Personal View" guid="{CD7B856B-9EDA-43C8-96C4-9EE3BFC6A1C7}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="592" tabRatio="602" activeSheetId="4"/>
-    <customWorkbookView name="Tatsiana Aleksina - Personal View" guid="{83803FE8-F026-4EB6-8AA8-850C4281E75D}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="588" tabRatio="602" activeSheetId="4"/>
-    <customWorkbookView name="Kathleen Walsh - Personal View" guid="{6C7C9A60-7A7A-4C49-B916-23929D5F2F41}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="643" tabRatio="602" activeSheetId="4" showFormulaBar="0"/>
-    <customWorkbookView name="Siarhei_Varanovich - Personal View" guid="{6243D704-9E25-11D6-9C67-009027ED19E6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="592" tabRatio="602" activeSheetId="3"/>
-    <customWorkbookView name="Siarhei_Serko - Personal View" guid="{CC0CF5D6-B18D-491A-9FC9-FEBD5F8814E3}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="580" tabRatio="608" activeSheetId="3"/>
-    <customWorkbookView name="Yuliya_Huziy - Personal View" guid="{FEF12470-2E23-407A-98E1-8AB431BD4F04}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="553" tabRatio="602" activeSheetId="4"/>
-    <customWorkbookView name="Alexandr Belousov - Personal View" guid="{EB2A7A54-3035-4A67-821E-790B1FA9CB17}" mergeInterval="0" personalView="1" maximized="1" xWindow="4" yWindow="100" windowWidth="1012" windowHeight="576" activeSheetId="3"/>
-    <customWorkbookView name="Andrei Kulabukhau - Personal View" guid="{4CB4A757-2DE4-4B10-9E8C-5353D1A72D98}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="579" activeSheetId="6"/>
-    <customWorkbookView name="Igor Kalnik - Personal View" guid="{ECDB2518-881D-11D6-91C5-00A0C96BDFA3}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="605" activeSheetId="3"/>
-    <customWorkbookView name="Tatsiana Bohush - Personal View" guid="{7BBCACAA-43E1-40B6-ADAE-BB35DF313022}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="632" activeSheetId="6"/>
-    <customWorkbookView name="Aliaksandra  Ivanova - Personal View" guid="{2B891D42-6CB2-11D6-83C8-0003470A98B2}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="581" tabRatio="608" activeSheetId="2"/>
-    <customWorkbookView name="Volha Bahachuk - Personal View" guid="{38F36526-3D5C-4DDC-870E-899FBC48B66E}" mergeInterval="0" personalView="1" maximized="1" xWindow="2" yWindow="96" windowWidth="1020" windowHeight="603" activeSheetId="3"/>
-    <customWorkbookView name="Alena  Yermokhina - Personal View" guid="{5B8FA0FD-6C82-11D6-82E3-00A0C9A45549}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="580" activeSheetId="3" showComments="commIndAndComment"/>
-    <customWorkbookView name="Ruslan Mianzelen - Personal View" guid="{56D8F5D9-3A0D-4BF2-9433-8BEFE08B3700}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="554" activeSheetId="3"/>
-    <customWorkbookView name="Aliaksandra V. Ivanova - Personal View" guid="{EFAB871B-4EC1-40A1-9A59-7F13D3251E5D}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="607" activeSheetId="2"/>
-    <customWorkbookView name="Developer - Personal View" guid="{F21FA1CE-8CDC-4011-8CB5-DD27B77A6F07}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="579" activeSheetId="7"/>
-    <customWorkbookView name="Aliaksandr Mamus - Personal View" guid="{FFC053D9-391A-4F3D-A4C4-D8F3DC5064CF}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1115" windowHeight="810" activeSheetId="3"/>
-    <customWorkbookView name="Pavel Drachuk - Personal View" guid="{3EDD5E41-79E4-11D6-8216-009027651E6D}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="581" activeSheetId="2"/>
-    <customWorkbookView name="Siarhei Varanovich - Personal View" guid="{33D53BDF-065D-44AA-B0C7-519973E98EF8}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="605" tabRatio="602" activeSheetId="3"/>
-    <customWorkbookView name="Tatsiana Alexina - Personal View" guid="{D717C572-E042-4CE9-8903-02D390043ABD}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="580" tabRatio="602" activeSheetId="3"/>
-    <customWorkbookView name="Andrei Savastsiuk - Personal View" guid="{E55FF256-6BD4-11D6-8424-009027ED1955}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="570" activeSheetId="3"/>
-    <customWorkbookView name="Andrei_Savastsiuk - Personal View" guid="{C303A572-AC36-442D-BA31-03981F899203}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="562" tabRatio="602" activeSheetId="1"/>
-    <customWorkbookView name="Dzmitry_Bachkarou - Personal View" guid="{C28FB00F-BF30-4FCE-8162-662CDD4F052E}" mergeInterval="0" personalView="1" maximized="1" windowWidth="868" windowHeight="577" tabRatio="602" activeSheetId="4"/>
-    <customWorkbookView name="Alena Yermokhina - Personal View" guid="{162B80D8-2A0E-434F-A609-2DA7C93548E1}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="859" tabRatio="602" activeSheetId="4"/>
-    <customWorkbookView name="Hanna_Shuminskaya - Personal View" guid="{7603C6CA-5974-4912-AE1D-2245B995DDB4}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="580" tabRatio="602" activeSheetId="4"/>
-    <customWorkbookView name="Katsiaryna_Yarshova - Personal View" guid="{D003CDB4-53EF-48AC-A14B-1EF99DCC6613}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="813" tabRatio="602" activeSheetId="1"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="147">
   <si>
     <t>Project Test</t>
   </si>
@@ -850,9 +850,6 @@
   </si>
   <si>
     <t>Link "Change your background image" is absent. Today Gmail using "Custom Themes"</t>
-  </si>
-  <si>
-    <t>Star label is absent. We can make it visible by changing settings.</t>
   </si>
 </sst>
 </file>
@@ -1002,7 +999,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1030,6 +1027,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1145,7 +1148,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1404,6 +1407,9 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1416,8 +1422,8 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1930,80 +1936,80 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{D6B20FFB-1E0B-461B-BCA5-479EC9916837}" showRuler="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <customSheetView guid="{D003CDB4-53EF-48AC-A14B-1EF99DCC6613}" showRuler="0">
+      <selection activeCell="B11" sqref="B11"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{CD7B856B-9EDA-43C8-96C4-9EE3BFC6A1C7}" showRuler="0">
+    <customSheetView guid="{7603C6CA-5974-4912-AE1D-2245B995DDB4}" showRuler="0">
       <selection activeCell="B13" sqref="B13"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{83803FE8-F026-4EB6-8AA8-850C4281E75D}" showRuler="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <customSheetView guid="{162B80D8-2A0E-434F-A609-2DA7C93548E1}" showRuler="0">
+      <selection activeCell="B13" sqref="B13"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{6C7C9A60-7A7A-4C49-B916-23929D5F2F41}" showRuler="0">
+    <customSheetView guid="{C28FB00F-BF30-4FCE-8162-662CDD4F052E}" showRuler="0">
       <selection activeCell="B13" sqref="B13"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId4"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{6243D704-9E25-11D6-9C67-009027ED19E6}" showRuler="0">
+    <customSheetView guid="{C303A572-AC36-442D-BA31-03981F899203}" showRuler="0">
+      <selection activeCell="A3" sqref="A3"/>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <pageSetup orientation="portrait" r:id="rId5"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
+    <customSheetView guid="{E55FF256-6BD4-11D6-8424-009027ED1955}" showPageBreaks="1" showRuler="0" topLeftCell="A4">
       <selection activeCell="B12" sqref="B12"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup orientation="portrait" r:id="rId5"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
-    <customSheetView guid="{CC0CF5D6-B18D-491A-9FC9-FEBD5F8814E3}" showRuler="0">
-      <selection activeCell="B9" sqref="B9"/>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup orientation="portrait" r:id="rId6"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
-    <customSheetView guid="{FEF12470-2E23-407A-98E1-8AB431BD4F04}" showRuler="0" topLeftCell="A4">
+      <pageSetup paperSize="9" orientation="landscape" r:id="rId6"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
+    <customSheetView guid="{D717C572-E042-4CE9-8903-02D390043ABD}" showRuler="0" topLeftCell="A4">
       <selection activeCell="B14" sqref="B14"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId7"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{EB2A7A54-3035-4A67-821E-790B1FA9CB17}" showPageBreaks="1" showRuler="0" topLeftCell="A4">
-      <selection activeCell="B3" sqref="B3"/>
+    <customSheetView guid="{33D53BDF-065D-44AA-B0C7-519973E98EF8}" showRuler="0">
+      <selection activeCell="B10" sqref="B10"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId8"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{4CB4A757-2DE4-4B10-9E8C-5353D1A72D98}" showRuler="0">
+    <customSheetView guid="{3EDD5E41-79E4-11D6-8216-009027651E6D}" showPageBreaks="1" showRuler="0">
+      <selection activeCell="C14" sqref="C14:C15"/>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <pageSetup orientation="portrait" r:id="rId9"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
+    <customSheetView guid="{FFC053D9-391A-4F3D-A4C4-D8F3DC5064CF}" showRuler="0">
+      <selection activeCell="B9" sqref="B9"/>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <pageSetup orientation="portrait" r:id="rId10"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
+    <customSheetView guid="{F21FA1CE-8CDC-4011-8CB5-DD27B77A6F07}" showRuler="0">
+      <selection activeCell="B9" sqref="B9"/>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <pageSetup orientation="portrait" r:id="rId11"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
+    <customSheetView guid="{EFAB871B-4EC1-40A1-9A59-7F13D3251E5D}" showPageBreaks="1" showRuler="0">
       <selection activeCell="B12" sqref="B12"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup orientation="portrait" r:id="rId9"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
-    <customSheetView guid="{ECDB2518-881D-11D6-91C5-00A0C96BDFA3}" showRuler="0" topLeftCell="A10">
-      <selection activeCell="A9" sqref="A9"/>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup orientation="portrait" r:id="rId10"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
-    <customSheetView guid="{7BBCACAA-43E1-40B6-ADAE-BB35DF313022}" showPageBreaks="1" showRuler="0" topLeftCell="A4">
-      <selection activeCell="B3" sqref="B3"/>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup orientation="portrait" r:id="rId11"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
-    <customSheetView guid="{2B891D42-6CB2-11D6-83C8-0003470A98B2}" showPageBreaks="1" showRuler="0" topLeftCell="A10">
+      <pageSetup orientation="portrait" r:id="rId12"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
+    <customSheetView guid="{56D8F5D9-3A0D-4BF2-9433-8BEFE08B3700}" showRuler="0">
       <selection activeCell="B9" sqref="B9"/>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup orientation="portrait" r:id="rId12"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
-    <customSheetView guid="{38F36526-3D5C-4DDC-870E-899FBC48B66E}" showRuler="0" topLeftCell="A10">
-      <selection activeCell="B13" sqref="B13"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId13"/>
       <headerFooter alignWithMargins="0"/>
@@ -2014,80 +2020,80 @@
       <pageSetup orientation="portrait" r:id="rId14"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{56D8F5D9-3A0D-4BF2-9433-8BEFE08B3700}" showRuler="0">
+    <customSheetView guid="{38F36526-3D5C-4DDC-870E-899FBC48B66E}" showRuler="0" topLeftCell="A10">
+      <selection activeCell="B13" sqref="B13"/>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <pageSetup orientation="portrait" r:id="rId15"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
+    <customSheetView guid="{2B891D42-6CB2-11D6-83C8-0003470A98B2}" showPageBreaks="1" showRuler="0" topLeftCell="A10">
       <selection activeCell="B9" sqref="B9"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup orientation="portrait" r:id="rId15"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
-    <customSheetView guid="{EFAB871B-4EC1-40A1-9A59-7F13D3251E5D}" showPageBreaks="1" showRuler="0">
+      <pageSetup orientation="portrait" r:id="rId16"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
+    <customSheetView guid="{7BBCACAA-43E1-40B6-ADAE-BB35DF313022}" showPageBreaks="1" showRuler="0" topLeftCell="A4">
+      <selection activeCell="B3" sqref="B3"/>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <pageSetup orientation="portrait" r:id="rId17"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
+    <customSheetView guid="{ECDB2518-881D-11D6-91C5-00A0C96BDFA3}" showRuler="0" topLeftCell="A10">
+      <selection activeCell="A9" sqref="A9"/>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <pageSetup orientation="portrait" r:id="rId18"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
+    <customSheetView guid="{4CB4A757-2DE4-4B10-9E8C-5353D1A72D98}" showRuler="0">
       <selection activeCell="B12" sqref="B12"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup orientation="portrait" r:id="rId16"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
-    <customSheetView guid="{F21FA1CE-8CDC-4011-8CB5-DD27B77A6F07}" showRuler="0">
-      <selection activeCell="B9" sqref="B9"/>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup orientation="portrait" r:id="rId17"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
-    <customSheetView guid="{FFC053D9-391A-4F3D-A4C4-D8F3DC5064CF}" showRuler="0">
-      <selection activeCell="B9" sqref="B9"/>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup orientation="portrait" r:id="rId18"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
-    <customSheetView guid="{3EDD5E41-79E4-11D6-8216-009027651E6D}" showPageBreaks="1" showRuler="0">
-      <selection activeCell="C14" sqref="C14:C15"/>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId19"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{33D53BDF-065D-44AA-B0C7-519973E98EF8}" showRuler="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <customSheetView guid="{EB2A7A54-3035-4A67-821E-790B1FA9CB17}" showPageBreaks="1" showRuler="0" topLeftCell="A4">
+      <selection activeCell="B3" sqref="B3"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId20"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{D717C572-E042-4CE9-8903-02D390043ABD}" showRuler="0" topLeftCell="A4">
+    <customSheetView guid="{FEF12470-2E23-407A-98E1-8AB431BD4F04}" showRuler="0" topLeftCell="A4">
       <selection activeCell="B14" sqref="B14"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId21"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{E55FF256-6BD4-11D6-8424-009027ED1955}" showPageBreaks="1" showRuler="0" topLeftCell="A4">
+    <customSheetView guid="{CC0CF5D6-B18D-491A-9FC9-FEBD5F8814E3}" showRuler="0">
+      <selection activeCell="B9" sqref="B9"/>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <pageSetup orientation="portrait" r:id="rId22"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
+    <customSheetView guid="{6243D704-9E25-11D6-9C67-009027ED19E6}" showRuler="0">
       <selection activeCell="B12" sqref="B12"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup paperSize="9" orientation="landscape" r:id="rId22"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
-    <customSheetView guid="{C303A572-AC36-442D-BA31-03981F899203}" showRuler="0">
-      <selection activeCell="A3" sqref="A3"/>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId23"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{C28FB00F-BF30-4FCE-8162-662CDD4F052E}" showRuler="0">
+    <customSheetView guid="{6C7C9A60-7A7A-4C49-B916-23929D5F2F41}" showRuler="0">
       <selection activeCell="B13" sqref="B13"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId24"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{162B80D8-2A0E-434F-A609-2DA7C93548E1}" showRuler="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <customSheetView guid="{83803FE8-F026-4EB6-8AA8-850C4281E75D}" showRuler="0">
+      <selection activeCell="B16" sqref="B16"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId25"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{7603C6CA-5974-4912-AE1D-2245B995DDB4}" showRuler="0">
+    <customSheetView guid="{CD7B856B-9EDA-43C8-96C4-9EE3BFC6A1C7}" showRuler="0">
       <selection activeCell="B13" sqref="B13"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId26"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{D003CDB4-53EF-48AC-A14B-1EF99DCC6613}" showRuler="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <customSheetView guid="{D6B20FFB-1E0B-461B-BCA5-479EC9916837}" showRuler="0">
+      <selection activeCell="B13" sqref="B13"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId27"/>
       <headerFooter alignWithMargins="0"/>
@@ -2108,8 +2114,8 @@
   </sheetPr>
   <dimension ref="A1:H80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="64" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="64" workbookViewId="0">
+      <selection activeCell="F73" sqref="F73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -2127,14 +2133,14 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:8" s="40" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="92" t="s">
+      <c r="A2" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
+      <c r="B2" s="93"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
       <c r="G2" s="28"/>
     </row>
     <row r="3" spans="1:8" s="33" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2459,7 +2465,7 @@
       <c r="E25" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="F25" s="93" t="s">
+      <c r="F25" s="94" t="s">
         <v>145</v>
       </c>
       <c r="G25" s="43"/>
@@ -2472,7 +2478,7 @@
         <v>60</v>
       </c>
       <c r="E26" s="46"/>
-      <c r="F26" s="94"/>
+      <c r="F26" s="95"/>
     </row>
     <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="49"/>
@@ -2484,7 +2490,7 @@
       <c r="E27" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="F27" s="94"/>
+      <c r="F27" s="95"/>
     </row>
     <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="49"/>
@@ -2496,7 +2502,7 @@
       <c r="E28" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="F28" s="94"/>
+      <c r="F28" s="95"/>
     </row>
     <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="49"/>
@@ -2506,7 +2512,7 @@
         <v>63</v>
       </c>
       <c r="E29" s="54"/>
-      <c r="F29" s="94"/>
+      <c r="F29" s="95"/>
     </row>
     <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="49"/>
@@ -2516,7 +2522,7 @@
         <v>64</v>
       </c>
       <c r="E30" s="54"/>
-      <c r="F30" s="94"/>
+      <c r="F30" s="95"/>
     </row>
     <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="49"/>
@@ -2526,7 +2532,7 @@
         <v>65</v>
       </c>
       <c r="E31" s="46"/>
-      <c r="F31" s="94"/>
+      <c r="F31" s="95"/>
     </row>
     <row r="32" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="49"/>
@@ -2536,7 +2542,7 @@
         <v>66</v>
       </c>
       <c r="E32" s="46"/>
-      <c r="F32" s="94"/>
+      <c r="F32" s="95"/>
     </row>
     <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A33" s="49"/>
@@ -2548,7 +2554,7 @@
       <c r="E33" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="F33" s="94"/>
+      <c r="F33" s="95"/>
     </row>
     <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="49"/>
@@ -2560,7 +2566,7 @@
       <c r="E34" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="F34" s="94"/>
+      <c r="F34" s="95"/>
     </row>
     <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" s="49"/>
@@ -2572,7 +2578,7 @@
       <c r="E35" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="F35" s="95"/>
+      <c r="F35" s="96"/>
     </row>
     <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A36" s="64"/>
@@ -2693,7 +2699,7 @@
     <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A46" s="78"/>
       <c r="B46" s="79"/>
-      <c r="C46" s="96"/>
+      <c r="C46" s="92"/>
       <c r="D46" s="81" t="s">
         <v>93</v>
       </c>
@@ -2703,7 +2709,7 @@
     <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A47" s="78"/>
       <c r="B47" s="79"/>
-      <c r="C47" s="96"/>
+      <c r="C47" s="92"/>
       <c r="D47" s="81" t="s">
         <v>94</v>
       </c>
@@ -2715,7 +2721,7 @@
     <row r="48" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A48" s="78"/>
       <c r="B48" s="79"/>
-      <c r="C48" s="96"/>
+      <c r="C48" s="92"/>
       <c r="D48" s="81" t="s">
         <v>95</v>
       </c>
@@ -2727,7 +2733,7 @@
     <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A49" s="78"/>
       <c r="B49" s="79"/>
-      <c r="C49" s="96"/>
+      <c r="C49" s="92"/>
       <c r="D49" s="81" t="s">
         <v>96</v>
       </c>
@@ -2739,7 +2745,7 @@
     <row r="50" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="78"/>
       <c r="B50" s="79"/>
-      <c r="C50" s="96"/>
+      <c r="C50" s="92"/>
       <c r="D50" s="81" t="s">
         <v>97</v>
       </c>
@@ -2749,7 +2755,7 @@
     <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A51" s="78"/>
       <c r="B51" s="79"/>
-      <c r="C51" s="96"/>
+      <c r="C51" s="92"/>
       <c r="D51" s="81" t="s">
         <v>98</v>
       </c>
@@ -2761,7 +2767,7 @@
     <row r="52" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A52" s="78"/>
       <c r="B52" s="79"/>
-      <c r="C52" s="96"/>
+      <c r="C52" s="92"/>
       <c r="D52" s="81" t="s">
         <v>99</v>
       </c>
@@ -2785,7 +2791,7 @@
     <row r="54" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A54" s="78"/>
       <c r="B54" s="79"/>
-      <c r="C54" s="96"/>
+      <c r="C54" s="92"/>
       <c r="D54" s="81" t="s">
         <v>93</v>
       </c>
@@ -2795,7 +2801,7 @@
     <row r="55" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A55" s="78"/>
       <c r="B55" s="79"/>
-      <c r="C55" s="96"/>
+      <c r="C55" s="92"/>
       <c r="D55" s="81" t="s">
         <v>94</v>
       </c>
@@ -2807,7 +2813,7 @@
     <row r="56" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A56" s="78"/>
       <c r="B56" s="79"/>
-      <c r="C56" s="96"/>
+      <c r="C56" s="92"/>
       <c r="D56" s="81" t="s">
         <v>105</v>
       </c>
@@ -2819,7 +2825,7 @@
     <row r="57" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A57" s="78"/>
       <c r="B57" s="79"/>
-      <c r="C57" s="96"/>
+      <c r="C57" s="92"/>
       <c r="D57" s="81" t="s">
         <v>106</v>
       </c>
@@ -2829,7 +2835,7 @@
     <row r="58" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A58" s="78"/>
       <c r="B58" s="79"/>
-      <c r="C58" s="96"/>
+      <c r="C58" s="92"/>
       <c r="D58" s="81" t="s">
         <v>107</v>
       </c>
@@ -2841,7 +2847,7 @@
     <row r="59" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A59" s="78"/>
       <c r="B59" s="79"/>
-      <c r="C59" s="96"/>
+      <c r="C59" s="92"/>
       <c r="D59" s="81" t="s">
         <v>108</v>
       </c>
@@ -3014,9 +3020,7 @@
       <c r="E73" s="81" t="s">
         <v>138</v>
       </c>
-      <c r="F73" s="90" t="s">
-        <v>147</v>
-      </c>
+      <c r="F73" s="97"/>
     </row>
     <row r="74" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A74" s="64"/>
@@ -3065,7 +3069,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{D6B20FFB-1E0B-461B-BCA5-479EC9916837}" showAutoFilter="1" hiddenRows="1" showRuler="0" topLeftCell="A142">
+    <customSheetView guid="{D003CDB4-53EF-48AC-A14B-1EF99DCC6613}" showAutoFilter="1" showRuler="0" topLeftCell="A142">
       <selection activeCell="A142" sqref="A142"/>
       <colBreaks count="5" manualBreakCount="5">
         <brk id="5" max="1048575" man="1"/>
@@ -3079,7 +3083,21 @@
       <headerFooter alignWithMargins="0"/>
       <autoFilter ref="B1:I1"/>
     </customSheetView>
-    <customSheetView guid="{CD7B856B-9EDA-43C8-96C4-9EE3BFC6A1C7}" showAutoFilter="1" showRuler="0" topLeftCell="A74">
+    <customSheetView guid="{7603C6CA-5974-4912-AE1D-2245B995DDB4}" showAutoFilter="1" hiddenRows="1" showRuler="0" topLeftCell="A142">
+      <selection activeCell="A142" sqref="A142"/>
+      <colBreaks count="5" manualBreakCount="5">
+        <brk id="5" max="1048575" man="1"/>
+        <brk id="8" max="1048575" man="1"/>
+        <brk id="11" max="1048575" man="1"/>
+        <brk id="13" max="1048575" man="1"/>
+        <brk id="24" max="1048575" man="1"/>
+      </colBreaks>
+      <pageMargins left="0.25" right="0.17" top="0.32" bottom="0.25" header="0.22" footer="0.17"/>
+      <pageSetup orientation="portrait" r:id="rId2"/>
+      <headerFooter alignWithMargins="0"/>
+      <autoFilter ref="B1:I1"/>
+    </customSheetView>
+    <customSheetView guid="{162B80D8-2A0E-434F-A609-2DA7C93548E1}" showAutoFilter="1" showRuler="0" topLeftCell="A74">
       <selection activeCell="A98" sqref="A98"/>
       <colBreaks count="5" manualBreakCount="5">
         <brk id="5" max="1048575" man="1"/>
@@ -3089,25 +3107,11 @@
         <brk id="24" max="1048575" man="1"/>
       </colBreaks>
       <pageMargins left="0.25" right="0.17" top="0.32" bottom="0.25" header="0.22" footer="0.17"/>
-      <pageSetup orientation="portrait" r:id="rId2"/>
+      <pageSetup orientation="portrait" r:id="rId3"/>
       <headerFooter alignWithMargins="0"/>
       <autoFilter ref="B1:I1"/>
     </customSheetView>
-    <customSheetView guid="{83803FE8-F026-4EB6-8AA8-850C4281E75D}" showAutoFilter="1" hiddenRows="1" showRuler="0" topLeftCell="A5">
-      <selection activeCell="D184" sqref="D184"/>
-      <colBreaks count="5" manualBreakCount="5">
-        <brk id="5" max="1048575" man="1"/>
-        <brk id="8" max="1048575" man="1"/>
-        <brk id="11" max="1048575" man="1"/>
-        <brk id="13" max="1048575" man="1"/>
-        <brk id="24" max="1048575" man="1"/>
-      </colBreaks>
-      <pageMargins left="0.25" right="0.17" top="0.32" bottom="0.25" header="0.22" footer="0.17"/>
-      <pageSetup orientation="portrait" r:id="rId3"/>
-      <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:I1"/>
-    </customSheetView>
-    <customSheetView guid="{6C7C9A60-7A7A-4C49-B916-23929D5F2F41}" showAutoFilter="1" showRuler="0" topLeftCell="A74">
+    <customSheetView guid="{C28FB00F-BF30-4FCE-8162-662CDD4F052E}" showAutoFilter="1" hiddenRows="1" showRuler="0" topLeftCell="A74">
       <selection activeCell="A98" sqref="A98"/>
       <colBreaks count="5" manualBreakCount="5">
         <brk id="5" max="1048575" man="1"/>
@@ -3121,8 +3125,8 @@
       <headerFooter alignWithMargins="0"/>
       <autoFilter ref="B1:I1"/>
     </customSheetView>
-    <customSheetView guid="{6243D704-9E25-11D6-9C67-009027ED19E6}" showAutoFilter="1" hiddenRows="1" showRuler="0" topLeftCell="C26">
-      <selection activeCell="G45" sqref="G45"/>
+    <customSheetView guid="{C303A572-AC36-442D-BA31-03981F899203}" showAutoFilter="1" hiddenRows="1" showRuler="0" topLeftCell="A4">
+      <selection activeCell="A213" sqref="A213"/>
       <colBreaks count="5" manualBreakCount="5">
         <brk id="5" max="1048575" man="1"/>
         <brk id="8" max="1048575" man="1"/>
@@ -3135,20 +3139,14 @@
       <headerFooter alignWithMargins="0"/>
       <autoFilter ref="B1:I1"/>
     </customSheetView>
-    <customSheetView guid="{CC0CF5D6-B18D-491A-9FC9-FEBD5F8814E3}" hiddenRows="1" showRuler="0" topLeftCell="A537">
-      <selection activeCell="C571" sqref="C571"/>
-      <colBreaks count="4" manualBreakCount="4">
-        <brk id="5" max="1048575" man="1"/>
-        <brk id="11" max="1048575" man="1"/>
-        <brk id="13" max="1048575" man="1"/>
-        <brk id="24" max="1048575" man="1"/>
-      </colBreaks>
-      <pageMargins left="0.25" right="0.17" top="0.32" bottom="0.25" header="0.22" footer="0.17"/>
-      <pageSetup orientation="portrait" r:id="rId6"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
-    <customSheetView guid="{FEF12470-2E23-407A-98E1-8AB431BD4F04}" hiddenRows="1" showRuler="0" topLeftCell="A221">
-      <selection activeCell="D701" sqref="D701"/>
+    <customSheetView guid="{E55FF256-6BD4-11D6-8424-009027ED1955}" showPageBreaks="1" hiddenRows="1" showRuler="0">
+      <selection activeCell="C7" sqref="C7"/>
+      <pageMargins left="0.23622047244094491" right="0" top="0.31496062992125984" bottom="0.23622047244094491" header="0.23622047244094491" footer="0.15748031496062992"/>
+      <pageSetup paperSize="9" orientation="landscape" r:id="rId6"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
+    <customSheetView guid="{D717C572-E042-4CE9-8903-02D390043ABD}" hiddenRows="1" showRuler="0">
+      <selection activeCell="A7" sqref="A7"/>
       <colBreaks count="4" manualBreakCount="4">
         <brk id="5" max="1048575" man="1"/>
         <brk id="11" max="1048575" man="1"/>
@@ -3159,69 +3157,42 @@
       <pageSetup orientation="portrait" r:id="rId7"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{EB2A7A54-3035-4A67-821E-790B1FA9CB17}" scale="75" showPageBreaks="1" showRuler="0" topLeftCell="A826">
-      <selection activeCell="G830" sqref="G830"/>
-      <colBreaks count="6" manualBreakCount="6">
+    <customSheetView guid="{33D53BDF-065D-44AA-B0C7-519973E98EF8}" hiddenRows="1" showRuler="0" topLeftCell="A408">
+      <selection activeCell="A691" activeCellId="1" sqref="A690 A691"/>
+      <colBreaks count="4" manualBreakCount="4">
         <brk id="5" max="1048575" man="1"/>
-        <brk id="9" max="1048575" man="1"/>
         <brk id="11" max="1048575" man="1"/>
         <brk id="13" max="1048575" man="1"/>
         <brk id="24" max="1048575" man="1"/>
-        <brk id="35" max="1048575" man="1"/>
       </colBreaks>
       <pageMargins left="0.25" right="0.25" top="0.32" bottom="0.25" header="0.22" footer="0.17"/>
       <pageSetup orientation="portrait" r:id="rId8"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{4CB4A757-2DE4-4B10-9E8C-5353D1A72D98}" scale="85" showRuler="0" topLeftCell="A763">
-      <selection activeCell="A1936" sqref="A1936:IV1936"/>
-      <colBreaks count="2" manualBreakCount="2">
+    <customSheetView guid="{3EDD5E41-79E4-11D6-8216-009027651E6D}" scale="75" showPageBreaks="1" hiddenRows="1" showRuler="0" topLeftCell="A822">
+      <selection activeCell="F836" sqref="F836"/>
+      <colBreaks count="5" manualBreakCount="5">
         <brk id="5" max="1048575" man="1"/>
-        <brk id="13" max="1048575" man="1"/>
+        <brk id="6" max="1048575" man="1"/>
+        <brk id="10" max="1048575" man="1"/>
+        <brk id="12" max="1048575" man="1"/>
+        <brk id="16" max="1048575" man="1"/>
       </colBreaks>
       <pageMargins left="0.25" right="0.25" top="0.32" bottom="0.25" header="0.22" footer="0.17"/>
       <pageSetup orientation="portrait" r:id="rId9"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{ECDB2518-881D-11D6-91C5-00A0C96BDFA3}" hiddenRows="1" showRuler="0" topLeftCell="A9">
-      <selection activeCell="A1106" sqref="A1106"/>
-      <colBreaks count="3" manualBreakCount="3">
+    <customSheetView guid="{FFC053D9-391A-4F3D-A4C4-D8F3DC5064CF}" showRuler="0" topLeftCell="A279">
+      <selection activeCell="E286" sqref="E286"/>
+      <colBreaks count="1" manualBreakCount="1">
         <brk id="5" max="1048575" man="1"/>
-        <brk id="11" max="1048575" man="1"/>
-        <brk id="13" max="1048575" man="1"/>
       </colBreaks>
       <pageMargins left="0.25" right="0.25" top="0.32" bottom="0.25" header="0.22" footer="0.17"/>
       <pageSetup orientation="portrait" r:id="rId10"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{7BBCACAA-43E1-40B6-ADAE-BB35DF313022}" showPageBreaks="1" showRuler="0" topLeftCell="A618">
-      <selection activeCell="H620" sqref="H620"/>
-      <colBreaks count="4" manualBreakCount="4">
-        <brk id="6" max="1048575" man="1"/>
-        <brk id="11" max="1048575" man="1"/>
-        <brk id="13" max="1048575" man="1"/>
-        <brk id="26" max="1048575" man="1"/>
-      </colBreaks>
-      <pageMargins left="0.25" right="0.25" top="0.32" bottom="0.25" header="0.22" footer="0.17"/>
-      <pageSetup scale="82" orientation="portrait" r:id="rId11"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
-    <customSheetView guid="{2B891D42-6CB2-11D6-83C8-0003470A98B2}" showPageBreaks="1" hiddenRows="1" showRuler="0" topLeftCell="A2301">
-      <selection activeCell="A2439" sqref="A2439:IV2439"/>
-      <colBreaks count="6" manualBreakCount="6">
-        <brk id="4" max="1048575" man="1"/>
-        <brk id="5" max="1048575" man="1"/>
-        <brk id="8" max="1048575" man="1"/>
-        <brk id="9" max="1048575" man="1"/>
-        <brk id="11" max="1048575" man="1"/>
-        <brk id="15" max="1048575" man="1"/>
-      </colBreaks>
-      <pageMargins left="0.25" right="0.25" top="0.32" bottom="0.25" header="0.22" footer="0.17"/>
-      <pageSetup orientation="portrait" r:id="rId12"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
-    <customSheetView guid="{38F36526-3D5C-4DDC-870E-899FBC48B66E}" hiddenRows="1" showRuler="0" topLeftCell="A2832">
-      <selection activeCell="C2833" sqref="C2833"/>
+    <customSheetView guid="{F21FA1CE-8CDC-4011-8CB5-DD27B77A6F07}" showPageBreaks="1" showRuler="0" topLeftCell="A2502">
+      <selection activeCell="B2506" sqref="B2506"/>
       <colBreaks count="5" manualBreakCount="5">
         <brk id="5" max="1048575" man="1"/>
         <brk id="9" max="1048575" man="1"/>
@@ -3230,8 +3201,57 @@
         <brk id="33" max="1048575" man="1"/>
       </colBreaks>
       <pageMargins left="0.25" right="0.25" top="0.32" bottom="0.25" header="0.22" footer="0.17"/>
+      <pageSetup orientation="portrait" r:id="rId11"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
+    <customSheetView guid="{EFAB871B-4EC1-40A1-9A59-7F13D3251E5D}" showPageBreaks="1" showRuler="0" topLeftCell="A2520">
+      <selection activeCell="A3027" sqref="A3027:IV3027"/>
+      <colBreaks count="5" manualBreakCount="5">
+        <brk id="3" max="1048575" man="1"/>
+        <brk id="4" max="1048575" man="1"/>
+        <brk id="8" max="1048575" man="1"/>
+        <brk id="10" max="1048575" man="1"/>
+        <brk id="12" max="1048575" man="1"/>
+      </colBreaks>
+      <pageMargins left="0.25" right="0.25" top="0.32" bottom="0.25" header="0.22" footer="0.17"/>
+      <pageSetup orientation="portrait" r:id="rId12"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
+    <customSheetView guid="{56D8F5D9-3A0D-4BF2-9433-8BEFE08B3700}" showPageBreaks="1" hiddenRows="1" showRuler="0" topLeftCell="A695">
+      <selection activeCell="D586" sqref="D586"/>
+      <colBreaks count="26" manualBreakCount="26">
+        <brk id="5" max="1048575" man="1"/>
+        <brk id="6" max="1048575" man="1"/>
+        <brk id="11" max="1048575" man="1"/>
+        <brk id="12" max="1048575" man="1"/>
+        <brk id="15" max="1048575" man="1"/>
+        <brk id="26" max="1992" man="1"/>
+        <brk id="37" max="1992" man="1"/>
+        <brk id="48" max="1992" man="1"/>
+        <brk id="59" max="1992" man="1"/>
+        <brk id="70" max="1992" man="1"/>
+        <brk id="81" max="1992" man="1"/>
+        <brk id="92" max="1992" man="1"/>
+        <brk id="103" max="1992" man="1"/>
+        <brk id="114" max="1992" man="1"/>
+        <brk id="125" max="1992" man="1"/>
+        <brk id="136" max="1992" man="1"/>
+        <brk id="147" max="1992" man="1"/>
+        <brk id="158" max="1992" man="1"/>
+        <brk id="169" max="1992" man="1"/>
+        <brk id="180" max="1992" man="1"/>
+        <brk id="191" max="1992" man="1"/>
+        <brk id="202" max="1992" man="1"/>
+        <brk id="213" max="1992" man="1"/>
+        <brk id="224" max="1992" man="1"/>
+        <brk id="235" max="1992" man="1"/>
+        <brk id="246" max="1992" man="1"/>
+      </colBreaks>
+      <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.31496062992125984" bottom="0.23622047244094491" header="0.15748031496062992" footer="0.15748031496062992"/>
       <pageSetup orientation="portrait" r:id="rId13"/>
-      <headerFooter alignWithMargins="0"/>
+      <headerFooter alignWithMargins="0">
+        <oddHeader>&amp;L&amp;D&amp;R&amp;P</oddHeader>
+      </headerFooter>
     </customSheetView>
     <customSheetView guid="{5B8FA0FD-6C82-11D6-82E3-00A0C9A45549}" showPageBreaks="1" hiddenRows="1" showRuler="0" topLeftCell="A1719">
       <selection activeCell="E1721" sqref="E1721"/>
@@ -3268,57 +3288,8 @@
         <oddHeader>&amp;L&amp;D&amp;R&amp;P</oddHeader>
       </headerFooter>
     </customSheetView>
-    <customSheetView guid="{56D8F5D9-3A0D-4BF2-9433-8BEFE08B3700}" showPageBreaks="1" hiddenRows="1" showRuler="0" topLeftCell="A695">
-      <selection activeCell="D586" sqref="D586"/>
-      <colBreaks count="26" manualBreakCount="26">
-        <brk id="5" max="1048575" man="1"/>
-        <brk id="6" max="1048575" man="1"/>
-        <brk id="11" max="1048575" man="1"/>
-        <brk id="12" max="1048575" man="1"/>
-        <brk id="15" max="1048575" man="1"/>
-        <brk id="26" max="1992" man="1"/>
-        <brk id="37" max="1992" man="1"/>
-        <brk id="48" max="1992" man="1"/>
-        <brk id="59" max="1992" man="1"/>
-        <brk id="70" max="1992" man="1"/>
-        <brk id="81" max="1992" man="1"/>
-        <brk id="92" max="1992" man="1"/>
-        <brk id="103" max="1992" man="1"/>
-        <brk id="114" max="1992" man="1"/>
-        <brk id="125" max="1992" man="1"/>
-        <brk id="136" max="1992" man="1"/>
-        <brk id="147" max="1992" man="1"/>
-        <brk id="158" max="1992" man="1"/>
-        <brk id="169" max="1992" man="1"/>
-        <brk id="180" max="1992" man="1"/>
-        <brk id="191" max="1992" man="1"/>
-        <brk id="202" max="1992" man="1"/>
-        <brk id="213" max="1992" man="1"/>
-        <brk id="224" max="1992" man="1"/>
-        <brk id="235" max="1992" man="1"/>
-        <brk id="246" max="1992" man="1"/>
-      </colBreaks>
-      <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.31496062992125984" bottom="0.23622047244094491" header="0.15748031496062992" footer="0.15748031496062992"/>
-      <pageSetup orientation="portrait" r:id="rId15"/>
-      <headerFooter alignWithMargins="0">
-        <oddHeader>&amp;L&amp;D&amp;R&amp;P</oddHeader>
-      </headerFooter>
-    </customSheetView>
-    <customSheetView guid="{EFAB871B-4EC1-40A1-9A59-7F13D3251E5D}" showPageBreaks="1" showRuler="0" topLeftCell="A2520">
-      <selection activeCell="A3027" sqref="A3027:IV3027"/>
-      <colBreaks count="5" manualBreakCount="5">
-        <brk id="3" max="1048575" man="1"/>
-        <brk id="4" max="1048575" man="1"/>
-        <brk id="8" max="1048575" man="1"/>
-        <brk id="10" max="1048575" man="1"/>
-        <brk id="12" max="1048575" man="1"/>
-      </colBreaks>
-      <pageMargins left="0.25" right="0.25" top="0.32" bottom="0.25" header="0.22" footer="0.17"/>
-      <pageSetup orientation="portrait" r:id="rId16"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
-    <customSheetView guid="{F21FA1CE-8CDC-4011-8CB5-DD27B77A6F07}" showPageBreaks="1" showRuler="0" topLeftCell="A2502">
-      <selection activeCell="B2506" sqref="B2506"/>
+    <customSheetView guid="{38F36526-3D5C-4DDC-870E-899FBC48B66E}" hiddenRows="1" showRuler="0" topLeftCell="A2832">
+      <selection activeCell="C2833" sqref="C2833"/>
       <colBreaks count="5" manualBreakCount="5">
         <brk id="5" max="1048575" man="1"/>
         <brk id="9" max="1048575" man="1"/>
@@ -3327,45 +3298,72 @@
         <brk id="33" max="1048575" man="1"/>
       </colBreaks>
       <pageMargins left="0.25" right="0.25" top="0.32" bottom="0.25" header="0.22" footer="0.17"/>
-      <pageSetup orientation="portrait" r:id="rId17"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
-    <customSheetView guid="{FFC053D9-391A-4F3D-A4C4-D8F3DC5064CF}" showRuler="0" topLeftCell="A279">
-      <selection activeCell="E286" sqref="E286"/>
-      <colBreaks count="1" manualBreakCount="1">
+      <pageSetup orientation="portrait" r:id="rId15"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
+    <customSheetView guid="{2B891D42-6CB2-11D6-83C8-0003470A98B2}" showPageBreaks="1" hiddenRows="1" showRuler="0" topLeftCell="A2301">
+      <selection activeCell="A2439" sqref="A2439:IV2439"/>
+      <colBreaks count="6" manualBreakCount="6">
+        <brk id="4" max="1048575" man="1"/>
         <brk id="5" max="1048575" man="1"/>
+        <brk id="8" max="1048575" man="1"/>
+        <brk id="9" max="1048575" man="1"/>
+        <brk id="11" max="1048575" man="1"/>
+        <brk id="15" max="1048575" man="1"/>
+      </colBreaks>
+      <pageMargins left="0.25" right="0.25" top="0.32" bottom="0.25" header="0.22" footer="0.17"/>
+      <pageSetup orientation="portrait" r:id="rId16"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
+    <customSheetView guid="{7BBCACAA-43E1-40B6-ADAE-BB35DF313022}" showPageBreaks="1" showRuler="0" topLeftCell="A618">
+      <selection activeCell="H620" sqref="H620"/>
+      <colBreaks count="4" manualBreakCount="4">
+        <brk id="6" max="1048575" man="1"/>
+        <brk id="11" max="1048575" man="1"/>
+        <brk id="13" max="1048575" man="1"/>
+        <brk id="26" max="1048575" man="1"/>
+      </colBreaks>
+      <pageMargins left="0.25" right="0.25" top="0.32" bottom="0.25" header="0.22" footer="0.17"/>
+      <pageSetup scale="82" orientation="portrait" r:id="rId17"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
+    <customSheetView guid="{ECDB2518-881D-11D6-91C5-00A0C96BDFA3}" hiddenRows="1" showRuler="0" topLeftCell="A9">
+      <selection activeCell="A1106" sqref="A1106"/>
+      <colBreaks count="3" manualBreakCount="3">
+        <brk id="5" max="1048575" man="1"/>
+        <brk id="11" max="1048575" man="1"/>
+        <brk id="13" max="1048575" man="1"/>
       </colBreaks>
       <pageMargins left="0.25" right="0.25" top="0.32" bottom="0.25" header="0.22" footer="0.17"/>
       <pageSetup orientation="portrait" r:id="rId18"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{3EDD5E41-79E4-11D6-8216-009027651E6D}" scale="75" showPageBreaks="1" hiddenRows="1" showRuler="0" topLeftCell="A822">
-      <selection activeCell="F836" sqref="F836"/>
-      <colBreaks count="5" manualBreakCount="5">
+    <customSheetView guid="{4CB4A757-2DE4-4B10-9E8C-5353D1A72D98}" scale="85" showRuler="0" topLeftCell="A763">
+      <selection activeCell="A1936" sqref="A1936:IV1936"/>
+      <colBreaks count="2" manualBreakCount="2">
         <brk id="5" max="1048575" man="1"/>
-        <brk id="6" max="1048575" man="1"/>
-        <brk id="10" max="1048575" man="1"/>
-        <brk id="12" max="1048575" man="1"/>
-        <brk id="16" max="1048575" man="1"/>
+        <brk id="13" max="1048575" man="1"/>
       </colBreaks>
       <pageMargins left="0.25" right="0.25" top="0.32" bottom="0.25" header="0.22" footer="0.17"/>
       <pageSetup orientation="portrait" r:id="rId19"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{33D53BDF-065D-44AA-B0C7-519973E98EF8}" hiddenRows="1" showRuler="0" topLeftCell="A408">
-      <selection activeCell="A691" activeCellId="1" sqref="A690 A691"/>
-      <colBreaks count="4" manualBreakCount="4">
+    <customSheetView guid="{EB2A7A54-3035-4A67-821E-790B1FA9CB17}" scale="75" showPageBreaks="1" showRuler="0" topLeftCell="A826">
+      <selection activeCell="G830" sqref="G830"/>
+      <colBreaks count="6" manualBreakCount="6">
         <brk id="5" max="1048575" man="1"/>
+        <brk id="9" max="1048575" man="1"/>
         <brk id="11" max="1048575" man="1"/>
         <brk id="13" max="1048575" man="1"/>
         <brk id="24" max="1048575" man="1"/>
+        <brk id="35" max="1048575" man="1"/>
       </colBreaks>
       <pageMargins left="0.25" right="0.25" top="0.32" bottom="0.25" header="0.22" footer="0.17"/>
       <pageSetup orientation="portrait" r:id="rId20"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{D717C572-E042-4CE9-8903-02D390043ABD}" hiddenRows="1" showRuler="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <customSheetView guid="{FEF12470-2E23-407A-98E1-8AB431BD4F04}" hiddenRows="1" showRuler="0" topLeftCell="A221">
+      <selection activeCell="D701" sqref="D701"/>
       <colBreaks count="4" manualBreakCount="4">
         <brk id="5" max="1048575" man="1"/>
         <brk id="11" max="1048575" man="1"/>
@@ -3376,14 +3374,20 @@
       <pageSetup orientation="portrait" r:id="rId21"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{E55FF256-6BD4-11D6-8424-009027ED1955}" showPageBreaks="1" hiddenRows="1" showRuler="0">
-      <selection activeCell="C7" sqref="C7"/>
-      <pageMargins left="0.23622047244094491" right="0" top="0.31496062992125984" bottom="0.23622047244094491" header="0.23622047244094491" footer="0.15748031496062992"/>
-      <pageSetup paperSize="9" orientation="landscape" r:id="rId22"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
-    <customSheetView guid="{C303A572-AC36-442D-BA31-03981F899203}" showAutoFilter="1" hiddenRows="1" showRuler="0" topLeftCell="A4">
-      <selection activeCell="A213" sqref="A213"/>
+    <customSheetView guid="{CC0CF5D6-B18D-491A-9FC9-FEBD5F8814E3}" hiddenRows="1" showRuler="0" topLeftCell="A537">
+      <selection activeCell="C571" sqref="C571"/>
+      <colBreaks count="4" manualBreakCount="4">
+        <brk id="5" max="1048575" man="1"/>
+        <brk id="11" max="1048575" man="1"/>
+        <brk id="13" max="1048575" man="1"/>
+        <brk id="24" max="1048575" man="1"/>
+      </colBreaks>
+      <pageMargins left="0.25" right="0.17" top="0.32" bottom="0.25" header="0.22" footer="0.17"/>
+      <pageSetup orientation="portrait" r:id="rId22"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
+    <customSheetView guid="{6243D704-9E25-11D6-9C67-009027ED19E6}" showAutoFilter="1" hiddenRows="1" showRuler="0" topLeftCell="C26">
+      <selection activeCell="G45" sqref="G45"/>
       <colBreaks count="5" manualBreakCount="5">
         <brk id="5" max="1048575" man="1"/>
         <brk id="8" max="1048575" man="1"/>
@@ -3396,7 +3400,7 @@
       <headerFooter alignWithMargins="0"/>
       <autoFilter ref="B1:I1"/>
     </customSheetView>
-    <customSheetView guid="{C28FB00F-BF30-4FCE-8162-662CDD4F052E}" showAutoFilter="1" hiddenRows="1" showRuler="0" topLeftCell="A74">
+    <customSheetView guid="{6C7C9A60-7A7A-4C49-B916-23929D5F2F41}" showAutoFilter="1" showRuler="0" topLeftCell="A74">
       <selection activeCell="A98" sqref="A98"/>
       <colBreaks count="5" manualBreakCount="5">
         <brk id="5" max="1048575" man="1"/>
@@ -3410,7 +3414,21 @@
       <headerFooter alignWithMargins="0"/>
       <autoFilter ref="B1:I1"/>
     </customSheetView>
-    <customSheetView guid="{162B80D8-2A0E-434F-A609-2DA7C93548E1}" showAutoFilter="1" showRuler="0" topLeftCell="A74">
+    <customSheetView guid="{83803FE8-F026-4EB6-8AA8-850C4281E75D}" showAutoFilter="1" hiddenRows="1" showRuler="0" topLeftCell="A5">
+      <selection activeCell="D184" sqref="D184"/>
+      <colBreaks count="5" manualBreakCount="5">
+        <brk id="5" max="1048575" man="1"/>
+        <brk id="8" max="1048575" man="1"/>
+        <brk id="11" max="1048575" man="1"/>
+        <brk id="13" max="1048575" man="1"/>
+        <brk id="24" max="1048575" man="1"/>
+      </colBreaks>
+      <pageMargins left="0.25" right="0.17" top="0.32" bottom="0.25" header="0.22" footer="0.17"/>
+      <pageSetup orientation="portrait" r:id="rId25"/>
+      <headerFooter alignWithMargins="0"/>
+      <autoFilter ref="B1:I1"/>
+    </customSheetView>
+    <customSheetView guid="{CD7B856B-9EDA-43C8-96C4-9EE3BFC6A1C7}" showAutoFilter="1" showRuler="0" topLeftCell="A74">
       <selection activeCell="A98" sqref="A98"/>
       <colBreaks count="5" manualBreakCount="5">
         <brk id="5" max="1048575" man="1"/>
@@ -3420,25 +3438,11 @@
         <brk id="24" max="1048575" man="1"/>
       </colBreaks>
       <pageMargins left="0.25" right="0.17" top="0.32" bottom="0.25" header="0.22" footer="0.17"/>
-      <pageSetup orientation="portrait" r:id="rId25"/>
+      <pageSetup orientation="portrait" r:id="rId26"/>
       <headerFooter alignWithMargins="0"/>
       <autoFilter ref="B1:I1"/>
     </customSheetView>
-    <customSheetView guid="{7603C6CA-5974-4912-AE1D-2245B995DDB4}" showAutoFilter="1" hiddenRows="1" showRuler="0" topLeftCell="A142">
-      <selection activeCell="A142" sqref="A142"/>
-      <colBreaks count="5" manualBreakCount="5">
-        <brk id="5" max="1048575" man="1"/>
-        <brk id="8" max="1048575" man="1"/>
-        <brk id="11" max="1048575" man="1"/>
-        <brk id="13" max="1048575" man="1"/>
-        <brk id="24" max="1048575" man="1"/>
-      </colBreaks>
-      <pageMargins left="0.25" right="0.17" top="0.32" bottom="0.25" header="0.22" footer="0.17"/>
-      <pageSetup orientation="portrait" r:id="rId26"/>
-      <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:I1"/>
-    </customSheetView>
-    <customSheetView guid="{D003CDB4-53EF-48AC-A14B-1EF99DCC6613}" showAutoFilter="1" showRuler="0" topLeftCell="A142">
+    <customSheetView guid="{D6B20FFB-1E0B-461B-BCA5-479EC9916837}" showAutoFilter="1" hiddenRows="1" showRuler="0" topLeftCell="A142">
       <selection activeCell="A142" sqref="A142"/>
       <colBreaks count="5" manualBreakCount="5">
         <brk id="5" max="1048575" man="1"/>

</xml_diff>